<commit_message>
Finalisation de la recuperation des cours
</commit_message>
<xml_diff>
--- a/src/main/resources/bourse.xlsx
+++ b/src/main/resources/bourse.xlsx
@@ -9,9 +9,9 @@
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="perso" sheetId="2" r:id="rId2"/>
+    <sheet name="graph" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:K17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="247">
   <si>
     <t>AXA</t>
   </si>
@@ -236,294 +236,195 @@
     <t>FR0000120628 CS</t>
   </si>
   <si>
-    <t>15,3080</t>
-  </si>
-  <si>
     <t>FR0000130809 GLE</t>
   </si>
   <si>
     <t>SOCIETE GENERALE</t>
   </si>
   <si>
-    <t>14,5860</t>
-  </si>
-  <si>
     <t>FR0000131104 BNP</t>
   </si>
   <si>
     <t>BNP PARIBAS</t>
   </si>
   <si>
-    <t>26,9550</t>
-  </si>
-  <si>
     <t>FR0000045072 ACA</t>
   </si>
   <si>
     <t>CREDIT AGRICOLE SA</t>
   </si>
   <si>
-    <t>6,7160</t>
-  </si>
-  <si>
     <t>FR0000120404 AC</t>
   </si>
   <si>
     <t>ACCOR</t>
   </si>
   <si>
-    <t>28,270</t>
-  </si>
-  <si>
     <t>FR0010208488 ENGI</t>
   </si>
   <si>
     <t>ENGIE</t>
   </si>
   <si>
-    <t>9,4220</t>
-  </si>
-  <si>
     <t>FR0000125007 SGO</t>
   </si>
   <si>
     <t>SAINT-GOBAIN</t>
   </si>
   <si>
-    <t>24,810</t>
-  </si>
-  <si>
     <t>AN8068571086 SLB</t>
   </si>
   <si>
     <t>SCHLUMBERGER</t>
   </si>
   <si>
-    <t>15,700</t>
-  </si>
-  <si>
     <t>US88579Y1010 MMM</t>
   </si>
   <si>
     <t>3M</t>
   </si>
   <si>
-    <t>149,040</t>
-  </si>
-  <si>
     <t>US0258161092 AXP</t>
   </si>
   <si>
     <t>AMERICAN EXPRESS</t>
   </si>
   <si>
-    <t>92,010</t>
-  </si>
-  <si>
     <t>US0378331005 AAPL</t>
   </si>
   <si>
     <t>APPLE</t>
   </si>
   <si>
-    <t>264,9100</t>
-  </si>
-  <si>
     <t>US1491231015 CATR</t>
   </si>
   <si>
     <t>CATERPILLAR</t>
   </si>
   <si>
-    <t>114,000</t>
-  </si>
-  <si>
     <t>US1667641005 CVX</t>
   </si>
   <si>
     <t>CHEVRON</t>
   </si>
   <si>
-    <t>85,190</t>
-  </si>
-  <si>
     <t>US17275R1023 CSCO</t>
   </si>
   <si>
     <t>CISCO SYSTEMS</t>
   </si>
   <si>
-    <t>41,5750</t>
-  </si>
-  <si>
     <t>US1912161007 KO</t>
   </si>
   <si>
     <t>COCA-COLA CO</t>
   </si>
   <si>
-    <t>48,000</t>
-  </si>
-  <si>
     <t>US2605571031 DOW</t>
   </si>
   <si>
     <t>DOW</t>
   </si>
   <si>
-    <t>34,730</t>
-  </si>
-  <si>
     <t>US30231G1022 XOM</t>
   </si>
   <si>
     <t>EXXON MOBIL</t>
   </si>
   <si>
-    <t>43,290</t>
-  </si>
-  <si>
     <t>US38141G1040 GS</t>
   </si>
   <si>
     <t>GOLDMAN SACHS GR</t>
   </si>
   <si>
-    <t>175,520</t>
-  </si>
-  <si>
     <t>US4370761029 HD</t>
   </si>
   <si>
     <t>HOME DEPOT</t>
   </si>
   <si>
-    <t>195,520</t>
-  </si>
-  <si>
     <t>US4592001014 IBM</t>
   </si>
   <si>
-    <t>119,289</t>
-  </si>
-  <si>
     <t>US4581401001 INTC</t>
   </si>
   <si>
     <t>INTEL</t>
   </si>
   <si>
-    <t>58,7450</t>
-  </si>
-  <si>
     <t>US46625H1005 JPM</t>
   </si>
   <si>
     <t>JPMORGAN CHASE</t>
   </si>
   <si>
-    <t>94,180</t>
-  </si>
-  <si>
     <t>US4781601046 JNJ</t>
   </si>
   <si>
     <t>JOHNSON&amp;JOHNSON</t>
   </si>
   <si>
-    <t>143,370</t>
-  </si>
-  <si>
     <t>US5801351017 MCD</t>
   </si>
   <si>
     <t>MCDONALD'S</t>
   </si>
   <si>
-    <t>176,630</t>
-  </si>
-  <si>
     <t>US6541061031 NKE</t>
   </si>
   <si>
     <t>NIKE -B-</t>
   </si>
   <si>
-    <t>85,600</t>
-  </si>
-  <si>
     <t>US7170811035 PFE</t>
   </si>
   <si>
     <t>PFIZER</t>
   </si>
   <si>
-    <t>34,655</t>
-  </si>
-  <si>
     <t>US7427181091 PG</t>
   </si>
   <si>
     <t>PROCTER&amp;GAMBLE</t>
   </si>
   <si>
-    <t>114,555</t>
-  </si>
-  <si>
     <t>US89417E1091 TRV</t>
   </si>
   <si>
     <t>TRAVELERS COS</t>
   </si>
   <si>
-    <t>104,660</t>
-  </si>
-  <si>
     <t>US9130171096 UTX</t>
   </si>
   <si>
     <t>UTD TECHS</t>
   </si>
   <si>
-    <t>86,140</t>
-  </si>
-  <si>
     <t>US92343V1044 VZ</t>
   </si>
   <si>
     <t>VERIZON COMM</t>
   </si>
   <si>
-    <t>57,728</t>
-  </si>
-  <si>
     <t>US92826C8394 V</t>
   </si>
   <si>
     <t>VISA RG-A</t>
   </si>
   <si>
-    <t>174,950</t>
-  </si>
-  <si>
     <t>US9314271084 WBA</t>
   </si>
   <si>
     <t>WALGREENS BOOTS</t>
   </si>
   <si>
-    <t>43,1600</t>
-  </si>
-  <si>
     <t>US2546871060 DIS</t>
   </si>
   <si>
     <t>WALT DISNEY</t>
   </si>
   <si>
-    <t>100,450</t>
-  </si>
-  <si>
     <t>indices</t>
   </si>
   <si>
@@ -554,22 +455,320 @@
     <t>Autres</t>
   </si>
   <si>
-    <t>AMD</t>
-  </si>
-  <si>
-    <t>LVMH</t>
-  </si>
-  <si>
     <t>https://www.boursorama.com/cours/1rPMC/</t>
   </si>
   <si>
     <t>https://www.boursorama.com/cours/AMD/</t>
+  </si>
+  <si>
+    <t>09/04/2020</t>
+  </si>
+  <si>
+    <t>US0079031078 AMD</t>
+  </si>
+  <si>
+    <t>ADVANCED MICRO D</t>
+  </si>
+  <si>
+    <t>FR0000121014 MC</t>
+  </si>
+  <si>
+    <t>LVMH MOET VUITTON</t>
+  </si>
+  <si>
+    <t>12/04/2020</t>
+  </si>
+  <si>
+    <t>14/04/2020</t>
+  </si>
+  <si>
+    <t>https://www.boursorama.com/cours/1rPAI/</t>
+  </si>
+  <si>
+    <t>https://www.boursorama.com/cours/1rPAIR/</t>
+  </si>
+  <si>
+    <t>https://www.boursorama.com/cours/1rPATO/</t>
+  </si>
+  <si>
+    <t>https://www.boursorama.com/cours/1rPEN/</t>
+  </si>
+  <si>
+    <t>https://www.boursorama.com/cours/1rPCAP/</t>
+  </si>
+  <si>
+    <t>https://www.boursorama.com/cours/1rPLR/</t>
+  </si>
+  <si>
+    <t>https://www.boursorama.com/cours/1rPOR/</t>
+  </si>
+  <si>
+    <t>https://www.boursorama.com/cours/1rPKER/</t>
+  </si>
+  <si>
+    <t>https://www.boursorama.com/cours/1rPRMS/</t>
+  </si>
+  <si>
+    <t>https://www.boursorama.com/cours/1rPEL/</t>
+  </si>
+  <si>
+    <t>https://www.boursorama.com/cours/1rPDSY/</t>
+  </si>
+  <si>
+    <t>https://www.boursorama.com/cours/1rPBN/</t>
+  </si>
+  <si>
+    <t>https://www.boursorama.com/cours/1rPCA/</t>
+  </si>
+  <si>
+    <t>https://www.boursorama.com/cours/1rPUG/</t>
+  </si>
+  <si>
+    <t>https://www.boursorama.com/cours/1rPRI/</t>
+  </si>
+  <si>
+    <t>https://www.boursorama.com/cours/1rPORA/</t>
+  </si>
+  <si>
+    <t>https://www.boursorama.com/cours/1rPML/</t>
+  </si>
+  <si>
+    <t>https://www.boursorama.com/cours/1rPPUB/</t>
+  </si>
+  <si>
+    <t>https://www.boursorama.com/cours/1rPRNO/</t>
+  </si>
+  <si>
+    <t>https://www.boursorama.com/cours/1rPSAF/</t>
+  </si>
+  <si>
+    <t>https://www.boursorama.com/cours/1rPSAN/</t>
+  </si>
+  <si>
+    <t>https://www.boursorama.com/cours/1rPSU/</t>
+  </si>
+  <si>
+    <t>https://www.boursorama.com/cours/1rPSW/</t>
+  </si>
+  <si>
+    <t>https://www.boursorama.com/cours/1rPSTM/</t>
+  </si>
+  <si>
+    <t>https://www.boursorama.com/cours/1rPHO/</t>
+  </si>
+  <si>
+    <t>https://www.boursorama.com/cours/1rPFP/</t>
+  </si>
+  <si>
+    <t>https://www.boursorama.com/cours/1rPVIE/</t>
+  </si>
+  <si>
+    <t>https://www.boursorama.com/cours/1rPDG/</t>
+  </si>
+  <si>
+    <t>https://www.boursorama.com/cours/1rPVIV/</t>
+  </si>
+  <si>
+    <t>https://www.boursorama.com/cours/1rPWLN/</t>
+  </si>
+  <si>
+    <t>15/04/2020</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>FR0011981968 WLN</t>
+  </si>
+  <si>
+    <t>WORLDLINE</t>
+  </si>
+  <si>
+    <t>FR0000127771 VIV</t>
+  </si>
+  <si>
+    <t>VIVENDI</t>
+  </si>
+  <si>
+    <t>FR0000125486 DG</t>
+  </si>
+  <si>
+    <t>VINCI</t>
+  </si>
+  <si>
+    <t>FR0000124141 VIE</t>
+  </si>
+  <si>
+    <t>VEOLIA ENVIRONNEM</t>
+  </si>
+  <si>
+    <t>FR0000120271 FP</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>FR0000121329 HO</t>
+  </si>
+  <si>
+    <t>THALES</t>
+  </si>
+  <si>
+    <t>NL0000226223 STM</t>
+  </si>
+  <si>
+    <t>STMICROELECTR</t>
+  </si>
+  <si>
+    <t>FR0000121220 SW</t>
+  </si>
+  <si>
+    <t>SODEXO</t>
+  </si>
+  <si>
+    <t>FR0000121972 SU</t>
+  </si>
+  <si>
+    <t>SCHNEIDER ELEC.</t>
+  </si>
+  <si>
+    <t>FR0000120578 SAN</t>
+  </si>
+  <si>
+    <t>SANOFI</t>
+  </si>
+  <si>
+    <t>FR0000073272 SAF</t>
+  </si>
+  <si>
+    <t>SAFRAN</t>
+  </si>
+  <si>
+    <t>FR0000131906 RNO</t>
+  </si>
+  <si>
+    <t>RENAULT</t>
+  </si>
+  <si>
+    <t>FR0000130577 PUB</t>
+  </si>
+  <si>
+    <t>PUBLICIS GRP</t>
+  </si>
+  <si>
+    <t>FR0000121261 ML</t>
+  </si>
+  <si>
+    <t>MICHELIN N</t>
+  </si>
+  <si>
+    <t>FR0000133308 ORA</t>
+  </si>
+  <si>
+    <t>ORANGE</t>
+  </si>
+  <si>
+    <t>FR0000120693 RI</t>
+  </si>
+  <si>
+    <t>PERNOD RICARD</t>
+  </si>
+  <si>
+    <t>FR0000121501 UG</t>
+  </si>
+  <si>
+    <t>PEUGEOT</t>
+  </si>
+  <si>
+    <t>FR0000120172 CA</t>
+  </si>
+  <si>
+    <t>CARREFOUR</t>
+  </si>
+  <si>
+    <t>FR0000120644 BN</t>
+  </si>
+  <si>
+    <t>DANONE</t>
+  </si>
+  <si>
+    <t>FR0000130650 DSY</t>
+  </si>
+  <si>
+    <t>DASSAULT SYSTEMES</t>
+  </si>
+  <si>
+    <t>FR0000121667 EL</t>
+  </si>
+  <si>
+    <t>ESSILORLUXOTTICA</t>
+  </si>
+  <si>
+    <t>FR0000052292 RMS</t>
+  </si>
+  <si>
+    <t>HERMES INTL</t>
+  </si>
+  <si>
+    <t>FR0000121485 KER</t>
+  </si>
+  <si>
+    <t>KERING</t>
+  </si>
+  <si>
+    <t>FR0000120321 OR</t>
+  </si>
+  <si>
+    <t>L'OREAL</t>
+  </si>
+  <si>
+    <t>FR0010307819 LR</t>
+  </si>
+  <si>
+    <t>LEGRAND</t>
+  </si>
+  <si>
+    <t>FR0000125338 CAP</t>
+  </si>
+  <si>
+    <t>CAPGEMINI</t>
+  </si>
+  <si>
+    <t>FR0000120503 EN</t>
+  </si>
+  <si>
+    <t>BOUYGUES</t>
+  </si>
+  <si>
+    <t>FR0000051732 ATO</t>
+  </si>
+  <si>
+    <t>ATOS</t>
+  </si>
+  <si>
+    <t>NL0000235190 AIR</t>
+  </si>
+  <si>
+    <t>AIRBUS</t>
+  </si>
+  <si>
+    <t>FR0000120073 AI</t>
+  </si>
+  <si>
+    <t>AIR LIQUIDE</t>
+  </si>
+  <si>
+    <t>16/04/2020</t>
+  </si>
+  <si>
+    <t>17/04/2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -608,13 +807,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -631,6 +831,655 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AXA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>data!$A$6:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>01/12/2019</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>08/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>09/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14/04/2020</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$B$6:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>24.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.308</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.311999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>15.53</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>15.587999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$C$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SOCIETE GENERALE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>data!$A$6:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>01/12/2019</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>08/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>09/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14/04/2020</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$C$6:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>28.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.586</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.728</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>15.022</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>15.066000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$D$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BNP PARIBAS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>data!$A$6:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>01/12/2019</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>08/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>09/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14/04/2020</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$D$6:$D$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>51.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.954999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28.1</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>28.405000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>28.29</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$E$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CREDIT AGRICOLE SA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>data!$A$6:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>01/12/2019</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>08/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>09/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14/04/2020</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$E$6:$E$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.7160000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.8819999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>6.9740000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>6.87</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$F$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ACCOR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>data!$A$6:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>01/12/2019</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>08/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>09/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14/04/2020</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$F$6:$F$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>38.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.27</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28.5</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>28.64</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>27.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$G$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ENGIE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>data!$A$6:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>01/12/2019</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>08/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>09/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14/04/2020</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$G$6:$G$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.4220000000000006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.6940000000000008</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>9.8859999999999992</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>9.7840000000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$H$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SAINT-GOBAIN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>data!$A$6:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>01/12/2019</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>08/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>09/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14/04/2020</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$H$6:$H$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>36.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.81</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25.63</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>25.98</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>25.57</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$I$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SCHLUMBERGER</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>data!$A$6:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>01/12/2019</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>08/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>09/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14/04/2020</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$I$6:$I$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>33.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>16.05</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>14.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="126934016"/>
+        <c:axId val="157175744"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="126934016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="157175744"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="157175744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="126934016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>504824</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -888,7 +1737,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -896,66 +1745,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ7"/>
+  <dimension ref="A1:BN20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AI8" sqref="AI8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="3"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" style="3" width="11.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="10" max="40" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>167</v>
+        <v>134</v>
       </c>
       <c r="B1" t="s">
-        <v>170</v>
-      </c>
-      <c r="J1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AO1" t="s">
         <v>9</v>
       </c>
-      <c r="AI1" t="s">
-        <v>176</v>
+      <c r="BN1" t="s">
+        <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>168</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
-        <v>169</v>
+        <v>136</v>
       </c>
       <c r="C2" t="s">
-        <v>169</v>
+        <v>136</v>
       </c>
       <c r="D2" t="s">
-        <v>169</v>
+        <v>136</v>
       </c>
       <c r="E2" t="s">
-        <v>169</v>
+        <v>136</v>
       </c>
       <c r="F2" t="s">
-        <v>169</v>
+        <v>136</v>
       </c>
       <c r="G2" t="s">
-        <v>169</v>
+        <v>136</v>
       </c>
       <c r="H2" t="s">
-        <v>169</v>
+        <v>136</v>
       </c>
       <c r="I2" t="s">
-        <v>169</v>
-      </c>
-      <c r="X2" t="s">
-        <v>175</v>
+        <v>136</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>66</v>
       </c>
@@ -983,89 +1833,179 @@
       <c r="I3" t="s">
         <v>8</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="Z3" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="AA3" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB3" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="AC3" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="AD3" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="AE3" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="AF3" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="AG3" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="AH3" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="AI3" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="AJ3" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="AK3" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="AL3" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="AM3" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="AN3" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="AO3" t="s">
         <v>11</v>
       </c>
-      <c r="K3" t="s">
+      <c r="AP3" t="s">
         <v>12</v>
       </c>
-      <c r="L3" t="s">
+      <c r="AQ3" t="s">
         <v>14</v>
       </c>
-      <c r="M3" t="s">
+      <c r="AR3" t="s">
         <v>13</v>
       </c>
-      <c r="N3" t="s">
+      <c r="AS3" t="s">
         <v>15</v>
       </c>
-      <c r="O3" t="s">
+      <c r="AT3" t="s">
         <v>16</v>
       </c>
-      <c r="P3" t="s">
+      <c r="AU3" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="AV3" t="s">
         <v>18</v>
       </c>
-      <c r="R3" t="s">
+      <c r="AW3" t="s">
         <v>19</v>
       </c>
-      <c r="S3" t="s">
+      <c r="AX3" t="s">
         <v>20</v>
       </c>
-      <c r="T3" t="s">
+      <c r="AY3" t="s">
         <v>21</v>
       </c>
-      <c r="U3" t="s">
+      <c r="AZ3" t="s">
         <v>22</v>
       </c>
-      <c r="V3" t="s">
+      <c r="BA3" t="s">
         <v>23</v>
       </c>
-      <c r="W3" t="s">
+      <c r="BB3" t="s">
         <v>24</v>
       </c>
-      <c r="X3" t="s">
+      <c r="BC3" t="s">
         <v>25</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="BD3" t="s">
         <v>26</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="BE3" t="s">
         <v>27</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="BF3" t="s">
         <v>28</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="BG3" t="s">
         <v>29</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="BH3" t="s">
         <v>30</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="BI3" t="s">
         <v>31</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="BJ3" t="s">
         <v>32</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="BK3" t="s">
         <v>33</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="BL3" t="s">
         <v>34</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="BM3" t="s">
         <v>35</v>
       </c>
-      <c r="AI3" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="AJ3" s="5" t="s">
-        <v>179</v>
+      <c r="BN3" s="5" t="s">
+        <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>67</v>
       </c>
@@ -1073,104 +2013,199 @@
         <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" t="s">
         <v>75</v>
       </c>
-      <c r="E4" t="s">
-        <v>78</v>
-      </c>
       <c r="F4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" t="s">
         <v>81</v>
       </c>
-      <c r="G4" t="s">
-        <v>84</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
+        <v>83</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="K4" t="s">
+        <v>185</v>
+      </c>
+      <c r="L4" t="s">
+        <v>187</v>
+      </c>
+      <c r="M4" t="s">
+        <v>189</v>
+      </c>
+      <c r="N4" t="s">
+        <v>191</v>
+      </c>
+      <c r="O4" t="s">
+        <v>193</v>
+      </c>
+      <c r="P4" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>197</v>
+      </c>
+      <c r="R4" t="s">
+        <v>199</v>
+      </c>
+      <c r="S4" t="s">
+        <v>201</v>
+      </c>
+      <c r="T4" t="s">
+        <v>203</v>
+      </c>
+      <c r="U4" t="s">
+        <v>205</v>
+      </c>
+      <c r="V4" t="s">
+        <v>207</v>
+      </c>
+      <c r="W4" t="s">
+        <v>209</v>
+      </c>
+      <c r="X4" t="s">
+        <v>211</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>213</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>217</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>219</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>221</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>223</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>225</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>227</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>229</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>231</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>233</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>235</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>239</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>241</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>243</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AP4" t="s">
         <v>87</v>
       </c>
-      <c r="I4" t="s">
-        <v>90</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="AQ4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AS4" t="s">
         <v>93</v>
       </c>
-      <c r="K4" t="s">
-        <v>96</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="AT4" t="s">
+        <v>95</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>97</v>
+      </c>
+      <c r="AV4" t="s">
         <v>99</v>
       </c>
-      <c r="M4" t="s">
-        <v>102</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="AW4" t="s">
+        <v>101</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>103</v>
+      </c>
+      <c r="AY4" t="s">
         <v>105</v>
       </c>
-      <c r="O4" t="s">
+      <c r="AZ4" t="s">
+        <v>107</v>
+      </c>
+      <c r="BA4" t="s">
         <v>108</v>
       </c>
-      <c r="P4" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="BB4" t="s">
+        <v>110</v>
+      </c>
+      <c r="BC4" t="s">
+        <v>112</v>
+      </c>
+      <c r="BD4" t="s">
         <v>114</v>
       </c>
-      <c r="R4" t="s">
-        <v>117</v>
-      </c>
-      <c r="S4" t="s">
+      <c r="BE4" t="s">
+        <v>116</v>
+      </c>
+      <c r="BF4" t="s">
+        <v>118</v>
+      </c>
+      <c r="BG4" t="s">
         <v>120</v>
       </c>
-      <c r="T4" t="s">
-        <v>123</v>
-      </c>
-      <c r="U4" t="s">
+      <c r="BH4" t="s">
+        <v>122</v>
+      </c>
+      <c r="BI4" t="s">
+        <v>124</v>
+      </c>
+      <c r="BJ4" t="s">
         <v>126</v>
       </c>
-      <c r="V4" t="s">
+      <c r="BK4" t="s">
         <v>128</v>
       </c>
-      <c r="W4" t="s">
-        <v>131</v>
-      </c>
-      <c r="X4" t="s">
-        <v>134</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>137</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>140</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>143</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>146</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>149</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>152</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>155</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>158</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>161</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>164</v>
-      </c>
-      <c r="AJ4" s="5"/>
+      <c r="BL4" t="s">
+        <v>130</v>
+      </c>
+      <c r="BM4" t="s">
+        <v>132</v>
+      </c>
+      <c r="BN4" t="s">
+        <v>147</v>
+      </c>
     </row>
-    <row r="5" spans="1:36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>68</v>
       </c>
@@ -1178,109 +2213,199 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" t="s">
         <v>76</v>
       </c>
-      <c r="E5" t="s">
-        <v>79</v>
-      </c>
       <c r="F5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" t="s">
         <v>82</v>
       </c>
-      <c r="G5" t="s">
-        <v>85</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
+        <v>84</v>
+      </c>
+      <c r="J5" t="s">
+        <v>150</v>
+      </c>
+      <c r="K5" t="s">
+        <v>186</v>
+      </c>
+      <c r="L5" t="s">
+        <v>188</v>
+      </c>
+      <c r="M5" t="s">
+        <v>190</v>
+      </c>
+      <c r="N5" t="s">
+        <v>192</v>
+      </c>
+      <c r="O5" t="s">
+        <v>194</v>
+      </c>
+      <c r="P5" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>198</v>
+      </c>
+      <c r="R5" t="s">
+        <v>200</v>
+      </c>
+      <c r="S5" t="s">
+        <v>202</v>
+      </c>
+      <c r="T5" t="s">
+        <v>204</v>
+      </c>
+      <c r="U5" t="s">
+        <v>206</v>
+      </c>
+      <c r="V5" t="s">
+        <v>208</v>
+      </c>
+      <c r="W5" t="s">
+        <v>210</v>
+      </c>
+      <c r="X5" t="s">
+        <v>212</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>214</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>216</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>218</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>220</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>222</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>224</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>226</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>228</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>230</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>232</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>234</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>236</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>238</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>240</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>242</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>244</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>86</v>
+      </c>
+      <c r="AP5" t="s">
         <v>88</v>
       </c>
-      <c r="I5" t="s">
-        <v>91</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="AQ5" t="s">
+        <v>90</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>92</v>
+      </c>
+      <c r="AS5" t="s">
         <v>94</v>
       </c>
-      <c r="K5" t="s">
-        <v>97</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="AT5" t="s">
+        <v>96</v>
+      </c>
+      <c r="AU5" t="s">
+        <v>98</v>
+      </c>
+      <c r="AV5" t="s">
         <v>100</v>
       </c>
-      <c r="M5" t="s">
-        <v>103</v>
-      </c>
-      <c r="N5" t="s">
+      <c r="AW5" t="s">
+        <v>102</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>104</v>
+      </c>
+      <c r="AY5" t="s">
         <v>106</v>
       </c>
-      <c r="O5" t="s">
+      <c r="AZ5" t="s">
+        <v>10</v>
+      </c>
+      <c r="BA5" t="s">
         <v>109</v>
       </c>
-      <c r="P5" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q5" t="s">
+      <c r="BB5" t="s">
+        <v>111</v>
+      </c>
+      <c r="BC5" t="s">
+        <v>113</v>
+      </c>
+      <c r="BD5" t="s">
         <v>115</v>
       </c>
-      <c r="R5" t="s">
-        <v>118</v>
-      </c>
-      <c r="S5" t="s">
+      <c r="BE5" t="s">
+        <v>117</v>
+      </c>
+      <c r="BF5" t="s">
+        <v>119</v>
+      </c>
+      <c r="BG5" t="s">
         <v>121</v>
       </c>
-      <c r="T5" t="s">
-        <v>124</v>
-      </c>
-      <c r="U5" t="s">
-        <v>10</v>
-      </c>
-      <c r="V5" t="s">
+      <c r="BH5" t="s">
+        <v>123</v>
+      </c>
+      <c r="BI5" t="s">
+        <v>125</v>
+      </c>
+      <c r="BJ5" t="s">
+        <v>127</v>
+      </c>
+      <c r="BK5" t="s">
         <v>129</v>
       </c>
-      <c r="W5" t="s">
-        <v>132</v>
-      </c>
-      <c r="X5" t="s">
-        <v>135</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>138</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>144</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>147</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>150</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>153</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>156</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>159</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>162</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>165</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>177</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>178</v>
+      <c r="BL5" t="s">
+        <v>131</v>
+      </c>
+      <c r="BM5" t="s">
+        <v>133</v>
+      </c>
+      <c r="BN5" t="s">
+        <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>43800</v>
       </c>
@@ -1309,198 +2434,1333 @@
         <v>33.1</v>
       </c>
       <c r="J6">
+        <v>408</v>
+      </c>
+      <c r="K6">
+        <v>58.8</v>
+      </c>
+      <c r="L6">
+        <v>24.97</v>
+      </c>
+      <c r="M6">
+        <v>98.9</v>
+      </c>
+      <c r="N6">
+        <v>23.26</v>
+      </c>
+      <c r="O6">
+        <v>47.69</v>
+      </c>
+      <c r="P6">
+        <v>89.12</v>
+      </c>
+      <c r="Q6">
+        <v>22.36</v>
+      </c>
+      <c r="R6">
+        <v>105.75</v>
+      </c>
+      <c r="S6">
+        <v>87.68</v>
+      </c>
+      <c r="T6">
+        <v>84.81</v>
+      </c>
+      <c r="U6">
+        <v>148.4</v>
+      </c>
+      <c r="V6">
+        <v>43.61</v>
+      </c>
+      <c r="W6">
+        <v>40.119999999999997</v>
+      </c>
+      <c r="X6">
+        <v>109.15</v>
+      </c>
+      <c r="Y6">
+        <v>14.8</v>
+      </c>
+      <c r="Z6">
+        <v>165.9</v>
+      </c>
+      <c r="AA6">
+        <v>21.99</v>
+      </c>
+      <c r="AB6">
+        <v>14.98</v>
+      </c>
+      <c r="AC6">
+        <v>74.8</v>
+      </c>
+      <c r="AD6">
+        <v>143</v>
+      </c>
+      <c r="AE6">
+        <v>141</v>
+      </c>
+      <c r="AF6">
+        <v>682</v>
+      </c>
+      <c r="AG6">
+        <v>546</v>
+      </c>
+      <c r="AH6">
+        <v>257.89999999999998</v>
+      </c>
+      <c r="AI6">
+        <v>71.680000000000007</v>
+      </c>
+      <c r="AJ6">
+        <v>107.35</v>
+      </c>
+      <c r="AK6">
+        <v>37.08</v>
+      </c>
+      <c r="AL6">
+        <v>77.099999999999994</v>
+      </c>
+      <c r="AM6">
+        <v>133.86000000000001</v>
+      </c>
+      <c r="AN6">
+        <v>122.8</v>
+      </c>
+      <c r="AO6">
         <v>170.2</v>
       </c>
-      <c r="K6">
+      <c r="AP6">
         <v>120</v>
       </c>
-      <c r="L6">
+      <c r="AQ6">
         <v>267.3</v>
       </c>
-      <c r="M6">
+      <c r="AR6">
         <v>133.5</v>
       </c>
-      <c r="N6">
+      <c r="AS6">
         <v>118</v>
       </c>
-      <c r="O6">
+      <c r="AT6">
         <v>45.2</v>
       </c>
-      <c r="P6">
+      <c r="AU6">
         <v>53.3</v>
       </c>
-      <c r="Q6">
+      <c r="AV6">
         <v>53</v>
       </c>
-      <c r="R6">
+      <c r="AW6">
         <v>68.400000000000006</v>
       </c>
-      <c r="S6">
+      <c r="AX6">
         <v>221</v>
       </c>
-      <c r="T6">
+      <c r="AY6">
         <v>220.7</v>
       </c>
-      <c r="U6">
+      <c r="AZ6">
         <v>134.5</v>
       </c>
-      <c r="V6">
+      <c r="BA6">
         <v>58.5</v>
       </c>
-      <c r="W6">
+      <c r="BB6">
         <v>132.30000000000001</v>
       </c>
-      <c r="X6">
+      <c r="BC6">
         <v>137.69999999999999</v>
       </c>
-      <c r="Y6">
+      <c r="BD6">
         <v>195.4</v>
       </c>
-      <c r="Z6">
+      <c r="BE6">
         <v>94</v>
       </c>
-      <c r="AA6">
+      <c r="BF6">
         <v>38.799999999999997</v>
       </c>
-      <c r="AB6">
+      <c r="BG6">
         <v>121.9</v>
       </c>
-      <c r="AC6">
+      <c r="BH6">
         <v>137</v>
       </c>
-      <c r="AD6">
+      <c r="BI6">
         <v>148.4</v>
       </c>
-      <c r="AE6">
+      <c r="BJ6">
         <v>60.2</v>
       </c>
-      <c r="AF6">
+      <c r="BK6">
         <v>184.1</v>
       </c>
-      <c r="AG6">
+      <c r="BL6">
         <v>59.3</v>
       </c>
-      <c r="AH6">
+      <c r="BM6">
         <v>147</v>
       </c>
-      <c r="AI6">
+      <c r="BN6">
         <v>39.36</v>
       </c>
     </row>
-    <row r="7" spans="1:36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>69</v>
       </c>
-      <c r="B7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C7" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E7" t="s">
-        <v>80</v>
-      </c>
-      <c r="F7" t="s">
-        <v>83</v>
-      </c>
-      <c r="G7" t="s">
-        <v>86</v>
-      </c>
-      <c r="H7" t="s">
-        <v>89</v>
-      </c>
-      <c r="I7" t="s">
-        <v>92</v>
-      </c>
-      <c r="J7" t="s">
-        <v>95</v>
-      </c>
-      <c r="K7" t="s">
-        <v>98</v>
-      </c>
-      <c r="L7" t="s">
-        <v>101</v>
-      </c>
-      <c r="M7" t="s">
-        <v>104</v>
-      </c>
-      <c r="N7" t="s">
-        <v>107</v>
-      </c>
-      <c r="O7" t="s">
-        <v>110</v>
-      </c>
-      <c r="P7" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q7" t="s">
+      <c r="B7" s="6">
+        <v>15.308</v>
+      </c>
+      <c r="C7" s="6">
+        <v>14.586</v>
+      </c>
+      <c r="D7" s="6">
+        <v>26.954999999999998</v>
+      </c>
+      <c r="E7" s="6">
+        <v>6.7160000000000002</v>
+      </c>
+      <c r="F7" s="6">
+        <v>28.27</v>
+      </c>
+      <c r="G7" s="6">
+        <v>9.4220000000000006</v>
+      </c>
+      <c r="H7" s="6">
+        <v>24.81</v>
+      </c>
+      <c r="I7" s="6">
+        <v>15.7</v>
+      </c>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="6"/>
+      <c r="AD7" s="6"/>
+      <c r="AE7" s="6"/>
+      <c r="AF7" s="6"/>
+      <c r="AG7" s="6"/>
+      <c r="AH7" s="6"/>
+      <c r="AI7" s="6"/>
+      <c r="AJ7" s="6"/>
+      <c r="AK7" s="6"/>
+      <c r="AL7" s="6"/>
+      <c r="AM7" s="6"/>
+      <c r="AN7" s="6"/>
+      <c r="AO7" s="6">
+        <v>149.04</v>
+      </c>
+      <c r="AP7" s="6">
+        <v>92.01</v>
+      </c>
+      <c r="AQ7" s="6">
+        <v>264.91000000000003</v>
+      </c>
+      <c r="AR7" s="6">
+        <v>114</v>
+      </c>
+      <c r="AS7" s="6">
+        <v>85.19</v>
+      </c>
+      <c r="AT7" s="6">
+        <v>41.575000000000003</v>
+      </c>
+      <c r="AU7" s="6">
+        <v>48</v>
+      </c>
+      <c r="AV7" s="6">
+        <v>34.729999999999997</v>
+      </c>
+      <c r="AW7" s="6">
+        <v>43.29</v>
+      </c>
+      <c r="AX7" s="6">
+        <v>175.52</v>
+      </c>
+      <c r="AY7" s="6">
+        <v>195.52</v>
+      </c>
+      <c r="AZ7" s="6">
+        <v>119.289</v>
+      </c>
+      <c r="BA7" s="6">
+        <v>58.744999999999997</v>
+      </c>
+      <c r="BB7" s="6">
+        <v>94.18</v>
+      </c>
+      <c r="BC7" s="6">
+        <v>143.37</v>
+      </c>
+      <c r="BD7" s="6">
+        <v>176.63</v>
+      </c>
+      <c r="BE7" s="6">
+        <v>85.6</v>
+      </c>
+      <c r="BF7" s="6">
+        <v>34.655000000000001</v>
+      </c>
+      <c r="BG7" s="6">
+        <v>114.55500000000001</v>
+      </c>
+      <c r="BH7" s="6">
+        <v>104.66</v>
+      </c>
+      <c r="BI7" s="6">
+        <v>86.14</v>
+      </c>
+      <c r="BJ7" s="6">
+        <v>57.728000000000002</v>
+      </c>
+      <c r="BK7" s="6">
+        <v>174.95</v>
+      </c>
+      <c r="BL7" s="6">
+        <v>43.16</v>
+      </c>
+      <c r="BM7" s="6">
+        <v>100.45</v>
+      </c>
+      <c r="BN7" s="6">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="8" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>146</v>
+      </c>
+      <c r="B8" s="6">
+        <v>15.311999999999999</v>
+      </c>
+      <c r="C8" s="6">
+        <v>14.728</v>
+      </c>
+      <c r="D8" s="6">
+        <v>28.1</v>
+      </c>
+      <c r="E8" s="6">
+        <v>6.8819999999999997</v>
+      </c>
+      <c r="F8" s="6">
+        <v>28.5</v>
+      </c>
+      <c r="G8" s="6">
+        <v>9.6940000000000008</v>
+      </c>
+      <c r="H8" s="6">
+        <v>25.63</v>
+      </c>
+      <c r="I8" s="6">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="J8" s="6">
+        <v>341.35</v>
+      </c>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="6"/>
+      <c r="AE8" s="6"/>
+      <c r="AF8" s="6"/>
+      <c r="AG8" s="6"/>
+      <c r="AH8" s="6"/>
+      <c r="AI8" s="6"/>
+      <c r="AJ8" s="6"/>
+      <c r="AK8" s="6"/>
+      <c r="AL8" s="6"/>
+      <c r="AM8" s="6"/>
+      <c r="AN8" s="6"/>
+      <c r="AO8" s="6">
+        <v>149.03</v>
+      </c>
+      <c r="AP8" s="6">
+        <v>92.03</v>
+      </c>
+      <c r="AQ8" s="6">
+        <v>266.07</v>
+      </c>
+      <c r="AR8" s="6">
+        <v>114</v>
+      </c>
+      <c r="AS8" s="6">
+        <v>86.04</v>
+      </c>
+      <c r="AT8" s="6">
+        <v>41.74</v>
+      </c>
+      <c r="AU8" s="6">
+        <v>47.78</v>
+      </c>
+      <c r="AV8" s="6">
+        <v>34.770000000000003</v>
+      </c>
+      <c r="AW8" s="6">
+        <v>43.86</v>
+      </c>
+      <c r="AX8" s="6">
+        <v>176.89</v>
+      </c>
+      <c r="AY8" s="6">
+        <v>194.6</v>
+      </c>
+      <c r="AZ8" s="6">
+        <v>119.28</v>
+      </c>
+      <c r="BA8" s="6">
+        <v>58.98</v>
+      </c>
+      <c r="BB8" s="6">
+        <v>94.25</v>
+      </c>
+      <c r="BC8" s="6">
+        <v>143.26</v>
+      </c>
+      <c r="BD8" s="6">
+        <v>177.42</v>
+      </c>
+      <c r="BE8" s="6">
+        <v>85.27</v>
+      </c>
+      <c r="BF8" s="6">
+        <v>34.619999999999997</v>
+      </c>
+      <c r="BG8" s="6">
+        <v>115.07</v>
+      </c>
+      <c r="BH8" s="6">
+        <v>104.91</v>
+      </c>
+      <c r="BI8" s="6">
+        <v>86.14</v>
+      </c>
+      <c r="BJ8" s="6">
+        <v>57.74</v>
+      </c>
+      <c r="BK8" s="6">
+        <v>174.81</v>
+      </c>
+      <c r="BL8" s="6">
+        <v>43.09</v>
+      </c>
+      <c r="BM8" s="6">
+        <v>101.01</v>
+      </c>
+      <c r="BN8" s="6">
+        <v>48.79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>151</v>
+      </c>
+      <c r="B9">
+        <v>15.53</v>
+      </c>
+      <c r="C9">
+        <v>15.022</v>
+      </c>
+      <c r="D9">
+        <v>28.405000000000001</v>
+      </c>
+      <c r="E9">
+        <v>6.9740000000000002</v>
+      </c>
+      <c r="F9">
+        <v>28.64</v>
+      </c>
+      <c r="G9">
+        <v>9.8859999999999992</v>
+      </c>
+      <c r="H9">
+        <v>25.98</v>
+      </c>
+      <c r="I9">
+        <v>16.05</v>
+      </c>
+      <c r="J9">
+        <v>347.4</v>
+      </c>
+      <c r="AO9">
+        <v>147.79</v>
+      </c>
+      <c r="AP9">
+        <v>94.79</v>
+      </c>
+      <c r="AQ9">
+        <v>267.99</v>
+      </c>
+      <c r="AR9">
+        <v>114</v>
+      </c>
+      <c r="AS9">
+        <v>84.34</v>
+      </c>
+      <c r="AT9">
+        <v>41.2</v>
+      </c>
+      <c r="AU9">
+        <v>48.98</v>
+      </c>
+      <c r="AV9">
+        <v>36.53</v>
+      </c>
+      <c r="AW9">
+        <v>43.08</v>
+      </c>
+      <c r="AX9">
+        <v>184.33</v>
+      </c>
+      <c r="AY9">
+        <v>201.41</v>
+      </c>
+      <c r="AZ9">
+        <v>121.37</v>
+      </c>
+      <c r="BA9">
+        <v>57.14</v>
+      </c>
+      <c r="BB9">
+        <v>102.74</v>
+      </c>
+      <c r="BC9">
+        <v>141.18</v>
+      </c>
+      <c r="BD9">
+        <v>183.67</v>
+      </c>
+      <c r="BE9">
+        <v>86.79</v>
+      </c>
+      <c r="BF9">
+        <v>35.380000000000003</v>
+      </c>
+      <c r="BG9">
+        <v>114.63</v>
+      </c>
+      <c r="BH9">
+        <v>109.66</v>
+      </c>
+      <c r="BI9">
+        <v>86.14</v>
+      </c>
+      <c r="BJ9">
+        <v>57.42</v>
+      </c>
+      <c r="BK9">
+        <v>173.68</v>
+      </c>
+      <c r="BL9">
+        <v>43.98</v>
+      </c>
+      <c r="BM9">
+        <v>104.5</v>
+      </c>
+      <c r="BN9">
+        <v>48.38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B10">
+        <v>15.587999999999999</v>
+      </c>
+      <c r="C10">
+        <v>15.066000000000001</v>
+      </c>
+      <c r="D10">
+        <v>28.29</v>
+      </c>
+      <c r="E10">
+        <v>6.87</v>
+      </c>
+      <c r="F10">
+        <v>27.8</v>
+      </c>
+      <c r="G10">
+        <v>9.7840000000000007</v>
+      </c>
+      <c r="H10">
+        <v>25.57</v>
+      </c>
+      <c r="I10">
+        <v>14.9</v>
+      </c>
+      <c r="J10">
+        <v>354.45</v>
+      </c>
+      <c r="AO10">
+        <v>146.31</v>
+      </c>
+      <c r="AP10">
+        <v>90.32</v>
+      </c>
+      <c r="AQ10">
+        <v>278.75</v>
+      </c>
+      <c r="AR10">
+        <v>114</v>
+      </c>
+      <c r="AS10">
+        <v>84.9</v>
+      </c>
+      <c r="AT10">
+        <v>41.22</v>
+      </c>
+      <c r="AU10">
+        <v>46.92</v>
+      </c>
+      <c r="AV10">
+        <v>35.22</v>
+      </c>
+      <c r="AW10">
+        <v>42.75</v>
+      </c>
+      <c r="AX10">
+        <v>179.39</v>
+      </c>
+      <c r="AY10">
+        <v>198.71</v>
+      </c>
+      <c r="AZ10">
+        <v>121.22</v>
+      </c>
+      <c r="BA10">
+        <v>58.7</v>
+      </c>
+      <c r="BB10">
+        <v>98.2</v>
+      </c>
+      <c r="BC10">
+        <v>139.97</v>
+      </c>
+      <c r="BD10">
+        <v>180.19</v>
+      </c>
+      <c r="BE10">
+        <v>84.42</v>
+      </c>
+      <c r="BF10">
+        <v>35.119999999999997</v>
+      </c>
+      <c r="BG10">
         <v>116</v>
       </c>
-      <c r="R7" t="s">
-        <v>119</v>
-      </c>
-      <c r="S7" t="s">
-        <v>122</v>
-      </c>
-      <c r="T7" t="s">
-        <v>125</v>
-      </c>
-      <c r="U7" t="s">
-        <v>127</v>
-      </c>
-      <c r="V7" t="s">
-        <v>130</v>
-      </c>
-      <c r="W7" t="s">
-        <v>133</v>
-      </c>
-      <c r="X7" t="s">
-        <v>136</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>139</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>142</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>145</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>148</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>151</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>154</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>157</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>160</v>
-      </c>
-      <c r="AG7" t="s">
-        <v>163</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>166</v>
-      </c>
-      <c r="AI7">
-        <v>408</v>
-      </c>
+      <c r="BH10">
+        <v>106.42</v>
+      </c>
+      <c r="BI10">
+        <v>86.14</v>
+      </c>
+      <c r="BJ10">
+        <v>56.66</v>
+      </c>
+      <c r="BK10">
+        <v>168.95</v>
+      </c>
+      <c r="BL10">
+        <v>45.057499999999997</v>
+      </c>
+      <c r="BM10">
+        <v>103.54</v>
+      </c>
+      <c r="BN10">
+        <v>52.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B11" t="n">
+        <v>15.002</v>
+      </c>
+      <c r="C11" t="n">
+        <v>13.934</v>
+      </c>
+      <c r="D11" t="n">
+        <v>26.56</v>
+      </c>
+      <c r="E11" t="n">
+        <v>6.468</v>
+      </c>
+      <c r="F11" t="n">
+        <v>25.67</v>
+      </c>
+      <c r="G11" t="n">
+        <v>9.538</v>
+      </c>
+      <c r="H11" t="n">
+        <v>24.05</v>
+      </c>
+      <c r="I11" t="n">
+        <v>13.95</v>
+      </c>
+      <c r="J11" t="n">
+        <v>346.5</v>
+      </c>
+      <c r="K11" t="n">
+        <v>58.44</v>
+      </c>
+      <c r="L11" t="n">
+        <v>20.82</v>
+      </c>
+      <c r="M11" t="n">
+        <v>74.04</v>
+      </c>
+      <c r="N11" t="n">
+        <v>18.925</v>
+      </c>
+      <c r="O11" t="n">
+        <v>30.895</v>
+      </c>
+      <c r="P11" t="n">
+        <v>70.36</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>21.14</v>
+      </c>
+      <c r="R11" t="n">
+        <v>66.42</v>
+      </c>
+      <c r="S11" t="n">
+        <v>80.72</v>
+      </c>
+      <c r="T11" t="n">
+        <v>84.48</v>
+      </c>
+      <c r="U11" t="n">
+        <v>75.86</v>
+      </c>
+      <c r="V11" t="n">
+        <v>17.136</v>
+      </c>
+      <c r="W11" t="n">
+        <v>28.52</v>
+      </c>
+      <c r="X11" t="n">
+        <v>84.42</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>11.435</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>137.9</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>12.21</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>14.215</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>61.74</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>132.95</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>106.35</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>676.4</v>
+      </c>
+      <c r="AG11" t="n">
+        <v>481.5</v>
+      </c>
+      <c r="AH11" t="n">
+        <v>253.9</v>
+      </c>
+      <c r="AI11" t="n">
+        <v>58.66</v>
+      </c>
+      <c r="AJ11" t="n">
+        <v>80.22</v>
+      </c>
+      <c r="AK11" t="n">
+        <v>27.74</v>
+      </c>
+      <c r="AL11" t="n">
+        <v>59.54</v>
+      </c>
+      <c r="AM11" t="n">
+        <v>57.18</v>
+      </c>
+      <c r="AN11" t="n">
+        <v>123.4</v>
+      </c>
+      <c r="AO11" t="n">
+        <v>150.13</v>
+      </c>
+      <c r="AP11" t="n">
+        <v>88.45</v>
+      </c>
+      <c r="AQ11" t="n">
+        <v>287.05</v>
+      </c>
+      <c r="AR11" t="n">
+        <v>106.0</v>
+      </c>
+      <c r="AS11" t="n">
+        <v>84.56</v>
+      </c>
+      <c r="AT11" t="n">
+        <v>42.78</v>
+      </c>
+      <c r="AU11" t="n">
+        <v>48.91</v>
+      </c>
+      <c r="AV11" t="n">
+        <v>35.39</v>
+      </c>
+      <c r="AW11" t="n">
+        <v>42.41</v>
+      </c>
+      <c r="AX11" t="n">
+        <v>178.32</v>
+      </c>
+      <c r="AY11" t="n">
+        <v>207.27</v>
+      </c>
+      <c r="AZ11" t="n">
+        <v>123.89</v>
+      </c>
+      <c r="BA11" t="n">
+        <v>60.66</v>
+      </c>
+      <c r="BB11" t="n">
+        <v>95.47</v>
+      </c>
+      <c r="BC11" t="n">
+        <v>145.98</v>
+      </c>
+      <c r="BD11" t="n">
+        <v>184.0</v>
+      </c>
+      <c r="BE11" t="n">
+        <v>87.49</v>
+      </c>
+      <c r="BF11" t="n">
+        <v>36.44</v>
+      </c>
+      <c r="BG11" t="n">
+        <v>120.99</v>
+      </c>
+      <c r="BH11" t="n">
+        <v>108.03</v>
+      </c>
+      <c r="BI11" t="n">
+        <v>86.14</v>
+      </c>
+      <c r="BJ11" t="n">
+        <v>58.12</v>
+      </c>
+      <c r="BK11" t="n">
+        <v>174.61</v>
+      </c>
+      <c r="BL11" t="n">
+        <v>46.38</v>
+      </c>
+      <c r="BM11" t="n">
+        <v>106.0</v>
+      </c>
+      <c r="BN11" t="n">
+        <v>54.93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="B12" t="n">
+        <v>14.656</v>
+      </c>
+      <c r="C12" t="n">
+        <v>13.402</v>
+      </c>
+      <c r="D12" t="n">
+        <v>25.48</v>
+      </c>
+      <c r="E12" t="n">
+        <v>6.28</v>
+      </c>
+      <c r="F12" t="n">
+        <v>24.88</v>
+      </c>
+      <c r="G12" t="n">
+        <v>9.312</v>
+      </c>
+      <c r="H12" t="n">
+        <v>24.24</v>
+      </c>
+      <c r="I12" t="n">
+        <v>13.85</v>
+      </c>
+      <c r="J12" t="n">
+        <v>344.05</v>
+      </c>
+      <c r="K12" t="n">
+        <v>56.76</v>
+      </c>
+      <c r="L12" t="n">
+        <v>20.41</v>
+      </c>
+      <c r="M12" t="n">
+        <v>72.56</v>
+      </c>
+      <c r="N12" t="n">
+        <v>19.35</v>
+      </c>
+      <c r="O12" t="n">
+        <v>30.53</v>
+      </c>
+      <c r="P12" t="n">
+        <v>68.92</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>20.84</v>
+      </c>
+      <c r="R12" t="n">
+        <v>62.32</v>
+      </c>
+      <c r="S12" t="n">
+        <v>79.7</v>
+      </c>
+      <c r="T12" t="n">
+        <v>84.41</v>
+      </c>
+      <c r="U12" t="n">
+        <v>75.96</v>
+      </c>
+      <c r="V12" t="n">
+        <v>16.548</v>
+      </c>
+      <c r="W12" t="n">
+        <v>26.51</v>
+      </c>
+      <c r="X12" t="n">
+        <v>82.42</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>11.185</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>135.95</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>11.635</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>13.95</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>61.64</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>138.85</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>108.45</v>
+      </c>
+      <c r="AF12" t="n">
+        <v>688.2</v>
+      </c>
+      <c r="AG12" t="n">
+        <v>481.9</v>
+      </c>
+      <c r="AH12" t="n">
+        <v>242.7</v>
+      </c>
+      <c r="AI12" t="n">
+        <v>57.46</v>
+      </c>
+      <c r="AJ12" t="n">
+        <v>78.52</v>
+      </c>
+      <c r="AK12" t="n">
+        <v>26.04</v>
+      </c>
+      <c r="AL12" t="n">
+        <v>59.48</v>
+      </c>
+      <c r="AM12" t="n">
+        <v>54.89</v>
+      </c>
+      <c r="AN12" t="n">
+        <v>121.0</v>
+      </c>
+      <c r="AO12" t="n">
+        <v>145.21</v>
+      </c>
+      <c r="AP12" t="n">
+        <v>83.79</v>
+      </c>
+      <c r="AQ12" t="n">
+        <v>284.43</v>
+      </c>
+      <c r="AR12" t="n">
+        <v>117.0</v>
+      </c>
+      <c r="AS12" t="n">
+        <v>82.52</v>
+      </c>
+      <c r="AT12" t="n">
+        <v>41.52</v>
+      </c>
+      <c r="AU12" t="n">
+        <v>47.61</v>
+      </c>
+      <c r="AV12" t="n">
+        <v>32.21</v>
+      </c>
+      <c r="AW12" t="n">
+        <v>40.51</v>
+      </c>
+      <c r="AX12" t="n">
+        <v>178.5</v>
+      </c>
+      <c r="AY12" t="n">
+        <v>198.51</v>
+      </c>
+      <c r="AZ12" t="n">
+        <v>118.69</v>
+      </c>
+      <c r="BA12" t="n">
+        <v>58.87</v>
+      </c>
+      <c r="BB12" t="n">
+        <v>90.82</v>
+      </c>
+      <c r="BC12" t="n">
+        <v>147.65</v>
+      </c>
+      <c r="BD12" t="n">
+        <v>177.725</v>
+      </c>
+      <c r="BE12" t="n">
+        <v>85.08</v>
+      </c>
+      <c r="BF12" t="n">
+        <v>35.98</v>
+      </c>
+      <c r="BG12" t="n">
+        <v>121.27</v>
+      </c>
+      <c r="BH12" t="n">
+        <v>102.23</v>
+      </c>
+      <c r="BI12" t="n">
+        <v>86.14</v>
+      </c>
+      <c r="BJ12" t="n">
+        <v>56.94</v>
+      </c>
+      <c r="BK12" t="n">
+        <v>165.96</v>
+      </c>
+      <c r="BL12" t="n">
+        <v>43.44</v>
+      </c>
+      <c r="BM12" t="n">
+        <v>103.38</v>
+      </c>
+      <c r="BN12" t="n">
+        <v>54.99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="B13" t="n">
+        <v>15.022</v>
+      </c>
+      <c r="C13" t="n">
+        <v>14.03</v>
+      </c>
+      <c r="D13" t="n">
+        <v>26.035</v>
+      </c>
+      <c r="E13" t="n">
+        <v>6.512</v>
+      </c>
+      <c r="F13" t="n">
+        <v>26.14</v>
+      </c>
+      <c r="G13" t="n">
+        <v>9.558</v>
+      </c>
+      <c r="H13" t="n">
+        <v>24.9</v>
+      </c>
+      <c r="I13" t="n">
+        <v>13.95</v>
+      </c>
+      <c r="J13" t="n">
+        <v>360.25</v>
+      </c>
+      <c r="K13" t="n">
+        <v>59.08</v>
+      </c>
+      <c r="L13" t="n">
+        <v>20.34</v>
+      </c>
+      <c r="M13" t="n">
+        <v>77.1</v>
+      </c>
+      <c r="N13" t="n">
+        <v>20.27</v>
+      </c>
+      <c r="O13" t="n">
+        <v>31.385</v>
+      </c>
+      <c r="P13" t="n">
+        <v>73.08</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>21.54</v>
+      </c>
+      <c r="R13" t="n">
+        <v>64.94</v>
+      </c>
+      <c r="S13" t="n">
+        <v>83.84</v>
+      </c>
+      <c r="T13" t="n">
+        <v>86.4</v>
+      </c>
+      <c r="U13" t="n">
+        <v>81.72</v>
+      </c>
+      <c r="V13" t="n">
+        <v>16.582</v>
+      </c>
+      <c r="W13" t="n">
+        <v>26.34</v>
+      </c>
+      <c r="X13" t="n">
+        <v>89.14</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>11.445</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>139.9</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>11.6</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>13.905</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>63.84</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>108.5</v>
+      </c>
+      <c r="AF13" t="n">
+        <v>686.6</v>
+      </c>
+      <c r="AG13" t="n">
+        <v>509.4</v>
+      </c>
+      <c r="AH13" t="n">
+        <v>250.3</v>
+      </c>
+      <c r="AI13" t="n">
+        <v>59.92</v>
+      </c>
+      <c r="AJ13" t="n">
+        <v>81.86</v>
+      </c>
+      <c r="AK13" t="n">
+        <v>26.99</v>
+      </c>
+      <c r="AL13" t="n">
+        <v>63.58</v>
+      </c>
+      <c r="AM13" t="n">
+        <v>57.57</v>
+      </c>
+      <c r="AN13" t="n">
+        <v>121.05</v>
+      </c>
+      <c r="AO13" t="n">
+        <v>144.86</v>
+      </c>
+      <c r="AP13" t="n">
+        <v>81.32</v>
+      </c>
+      <c r="AQ13" t="n">
+        <v>286.69</v>
+      </c>
+      <c r="AR13" t="n">
+        <v>106.0</v>
+      </c>
+      <c r="AS13" t="n">
+        <v>80.0</v>
+      </c>
+      <c r="AT13" t="n">
+        <v>41.5</v>
+      </c>
+      <c r="AU13" t="n">
+        <v>47.1</v>
+      </c>
+      <c r="AV13" t="n">
+        <v>31.62</v>
+      </c>
+      <c r="AW13" t="n">
+        <v>39.14</v>
+      </c>
+      <c r="AX13" t="n">
+        <v>177.03</v>
+      </c>
+      <c r="AY13" t="n">
+        <v>199.84</v>
+      </c>
+      <c r="AZ13" t="n">
+        <v>115.69</v>
+      </c>
+      <c r="BA13" t="n">
+        <v>60.79</v>
+      </c>
+      <c r="BB13" t="n">
+        <v>87.32</v>
+      </c>
+      <c r="BC13" t="n">
+        <v>149.74</v>
+      </c>
+      <c r="BD13" t="n">
+        <v>179.51</v>
+      </c>
+      <c r="BE13" t="n">
+        <v>86.3</v>
+      </c>
+      <c r="BF13" t="n">
+        <v>35.93</v>
+      </c>
+      <c r="BG13" t="n">
+        <v>121.54</v>
+      </c>
+      <c r="BH13" t="n">
+        <v>99.8</v>
+      </c>
+      <c r="BI13" t="n">
+        <v>86.14</v>
+      </c>
+      <c r="BJ13" t="n">
+        <v>57.68</v>
+      </c>
+      <c r="BK13" t="n">
+        <v>162.41</v>
+      </c>
+      <c r="BL13" t="n">
+        <v>43.23</v>
+      </c>
+      <c r="BM13" t="n">
+        <v>101.99</v>
+      </c>
+      <c r="BN13" t="n">
+        <v>56.95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+    </row>
+    <row r="15" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+    </row>
+    <row r="16" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AJ3" r:id="rId1"/>
-    <hyperlink ref="AI3" r:id="rId2"/>
+    <hyperlink ref="J3" r:id="rId1"/>
+    <hyperlink ref="BN3" r:id="rId2"/>
+    <hyperlink ref="AN3" r:id="rId3"/>
+    <hyperlink ref="AM3" r:id="rId4"/>
+    <hyperlink ref="AL3" r:id="rId5"/>
+    <hyperlink ref="AK3" r:id="rId6"/>
+    <hyperlink ref="AJ3" r:id="rId7"/>
+    <hyperlink ref="AI3" r:id="rId8"/>
+    <hyperlink ref="AH3" r:id="rId9"/>
+    <hyperlink ref="AG3" r:id="rId10"/>
+    <hyperlink ref="AF3" r:id="rId11"/>
+    <hyperlink ref="AE3" r:id="rId12"/>
+    <hyperlink ref="AD3" r:id="rId13"/>
+    <hyperlink ref="AC3" r:id="rId14"/>
+    <hyperlink ref="AB3" r:id="rId15"/>
+    <hyperlink ref="AA3" r:id="rId16"/>
+    <hyperlink ref="Z3" r:id="rId17"/>
+    <hyperlink ref="Y3" r:id="rId18"/>
+    <hyperlink ref="X3" r:id="rId19"/>
+    <hyperlink ref="W3" r:id="rId20"/>
+    <hyperlink ref="V3" r:id="rId21"/>
+    <hyperlink ref="U3" r:id="rId22"/>
+    <hyperlink ref="T3" r:id="rId23"/>
+    <hyperlink ref="S3" r:id="rId24"/>
+    <hyperlink ref="R3" r:id="rId25"/>
+    <hyperlink ref="Q3" r:id="rId26"/>
+    <hyperlink ref="P3" r:id="rId27"/>
+    <hyperlink ref="O3" r:id="rId28"/>
+    <hyperlink ref="N3" r:id="rId29"/>
+    <hyperlink ref="M3" r:id="rId30"/>
+    <hyperlink ref="L3" r:id="rId31"/>
+    <hyperlink ref="K3" r:id="rId32"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId33"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;10&amp;K0078D7C1 - Interne</oddFooter>
   </headerFooter>
@@ -1734,25 +3994,40 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>171</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>172</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>173</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>174</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Reorg pour pouvoir faire l'analyser
</commit_message>
<xml_diff>
--- a/src/main/resources/bourse.xlsx
+++ b/src/main/resources/bourse.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="13995" windowHeight="5610" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="13995" windowHeight="5610" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="252">
   <si>
     <t>AXA</t>
   </si>
@@ -761,12 +761,31 @@
   </si>
   <si>
     <t>17/04/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>diff from ref (%)</t>
+  </si>
+  <si>
+    <t>% ref</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>% 1 week</t>
+  </si>
+  <si>
+    <t>% 2 days</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -805,7 +824,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="403">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -813,6 +832,402 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1533,11 +1948,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="190590464"/>
-        <c:axId val="159928256"/>
+        <c:axId val="193041408"/>
+        <c:axId val="161371200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="190590464"/>
+        <c:axId val="193041408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1546,7 +1961,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159928256"/>
+        <c:crossAx val="161371200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1554,7 +1969,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="159928256"/>
+        <c:axId val="161371200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1565,14 +1980,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190590464"/>
+        <c:crossAx val="193041408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1879,7 +2293,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1895,9 +2309,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="3" collapsed="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="40" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" style="3" width="11.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="9" max="40" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:66" x14ac:dyDescent="0.25">
@@ -3910,13 +4324,937 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+      <c r="B1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="238" t="n">
+        <v>-0.39</v>
+      </c>
+      <c r="C2" t="n" s="239">
+        <v>-0.02</v>
+      </c>
+      <c r="D2" t="n" s="240">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="241" t="n">
+        <v>-0.51</v>
+      </c>
+      <c r="C3" t="n" s="242">
+        <v>-0.05</v>
+      </c>
+      <c r="D3" t="n" s="243">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="244" t="n">
+        <v>-0.49</v>
+      </c>
+      <c r="C4" t="n" s="245">
+        <v>-0.07</v>
+      </c>
+      <c r="D4" t="n" s="246">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="247" t="n">
+        <v>-0.48</v>
+      </c>
+      <c r="C5" t="n" s="248">
+        <v>-0.05</v>
+      </c>
+      <c r="D5" t="n" s="249">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="250" t="n">
+        <v>-0.33</v>
+      </c>
+      <c r="C6" t="n" s="251">
+        <v>-0.08</v>
+      </c>
+      <c r="D6" t="n" s="252">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="253" t="n">
+        <v>-0.34</v>
+      </c>
+      <c r="C7" t="n" s="254">
+        <v>-0.01</v>
+      </c>
+      <c r="D7" t="n" s="255">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="256" t="n">
+        <v>-0.32</v>
+      </c>
+      <c r="C8" t="n" s="257">
+        <v>-0.03</v>
+      </c>
+      <c r="D8" t="n" s="258">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="259" t="n">
+        <v>-0.58</v>
+      </c>
+      <c r="C9" t="n" s="260">
+        <v>-0.15</v>
+      </c>
+      <c r="D9" t="n" s="261">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10" s="262" t="n">
+        <v>-0.12</v>
+      </c>
+      <c r="C10" t="n" s="263">
+        <v>0.06</v>
+      </c>
+      <c r="D10" t="n" s="264">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>185</v>
+      </c>
+      <c r="B11" s="265" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>249</v>
+      </c>
+      <c r="D11" t="n" s="266">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>187</v>
+      </c>
+      <c r="B12" s="267" t="n">
+        <v>-0.19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>249</v>
+      </c>
+      <c r="D12" t="n" s="268">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>189</v>
+      </c>
+      <c r="B13" s="269" t="n">
+        <v>-0.22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>249</v>
+      </c>
+      <c r="D13" t="n" s="270">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>191</v>
+      </c>
+      <c r="B14" s="271" t="n">
+        <v>-0.13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>249</v>
+      </c>
+      <c r="D14" t="n" s="272">
+        <v>0.07</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>193</v>
+      </c>
+      <c r="B15" s="273" t="n">
+        <v>-0.34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>249</v>
+      </c>
+      <c r="D15" t="n" s="274">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>195</v>
+      </c>
+      <c r="B16" s="275" t="n">
+        <v>-0.18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>249</v>
+      </c>
+      <c r="D16" t="n" s="276">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>197</v>
+      </c>
+      <c r="B17" s="277" t="n">
+        <v>-0.04</v>
+      </c>
+      <c r="C17" t="s">
+        <v>249</v>
+      </c>
+      <c r="D17" t="n" s="278">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>199</v>
+      </c>
+      <c r="B18" s="279" t="n">
+        <v>-0.39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>249</v>
+      </c>
+      <c r="D18" t="n" s="280">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>201</v>
+      </c>
+      <c r="B19" s="281" t="n">
+        <v>-0.04</v>
+      </c>
+      <c r="C19" t="s">
+        <v>249</v>
+      </c>
+      <c r="D19" t="n" s="282">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>203</v>
+      </c>
+      <c r="B20" s="283" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="C20" t="s">
+        <v>249</v>
+      </c>
+      <c r="D20" t="n" s="284">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>205</v>
+      </c>
+      <c r="B21" s="285" t="n">
+        <v>-0.45</v>
+      </c>
+      <c r="C21" t="s">
+        <v>249</v>
+      </c>
+      <c r="D21" t="n" s="286">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>207</v>
+      </c>
+      <c r="B22" s="287" t="n">
+        <v>-0.62</v>
+      </c>
+      <c r="C22" t="s">
+        <v>249</v>
+      </c>
+      <c r="D22" t="n" s="288">
+        <v>-0.03</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>209</v>
+      </c>
+      <c r="B23" s="289" t="n">
+        <v>-0.34</v>
+      </c>
+      <c r="C23" t="s">
+        <v>249</v>
+      </c>
+      <c r="D23" t="n" s="290">
+        <v>-0.08</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>211</v>
+      </c>
+      <c r="B24" s="291" t="n">
+        <v>-0.18</v>
+      </c>
+      <c r="C24" t="s">
+        <v>249</v>
+      </c>
+      <c r="D24" t="n" s="292">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>213</v>
+      </c>
+      <c r="B25" s="293" t="n">
+        <v>-0.23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>249</v>
+      </c>
+      <c r="D25" t="n" s="294">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>215</v>
+      </c>
+      <c r="B26" s="295" t="n">
+        <v>-0.16</v>
+      </c>
+      <c r="C26" t="s">
+        <v>249</v>
+      </c>
+      <c r="D26" t="n" s="296">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>217</v>
+      </c>
+      <c r="B27" s="297" t="n">
+        <v>-0.47</v>
+      </c>
+      <c r="C27" t="s">
+        <v>249</v>
+      </c>
+      <c r="D27" t="n" s="298">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>219</v>
+      </c>
+      <c r="B28" s="299" t="n">
+        <v>-0.07</v>
+      </c>
+      <c r="C28" t="s">
+        <v>249</v>
+      </c>
+      <c r="D28" t="n" s="300">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>221</v>
+      </c>
+      <c r="B29" s="301" t="n">
+        <v>-0.15</v>
+      </c>
+      <c r="C29" t="s">
+        <v>249</v>
+      </c>
+      <c r="D29" t="n" s="302">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>223</v>
+      </c>
+      <c r="B30" s="303" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="C30" t="s">
+        <v>249</v>
+      </c>
+      <c r="D30" t="n" s="304">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>225</v>
+      </c>
+      <c r="B31" s="305" t="n">
+        <v>-0.23</v>
+      </c>
+      <c r="C31" t="s">
+        <v>249</v>
+      </c>
+      <c r="D31" t="n" s="306">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>227</v>
+      </c>
+      <c r="B32" s="307" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C32" t="s">
+        <v>249</v>
+      </c>
+      <c r="D32" t="n" s="308">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>229</v>
+      </c>
+      <c r="B33" s="309" t="n">
+        <v>-0.07</v>
+      </c>
+      <c r="C33" t="s">
+        <v>249</v>
+      </c>
+      <c r="D33" t="n" s="310">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>231</v>
+      </c>
+      <c r="B34" s="311" t="n">
+        <v>-0.03</v>
+      </c>
+      <c r="C34" t="s">
+        <v>249</v>
+      </c>
+      <c r="D34" t="n" s="312">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>233</v>
+      </c>
+      <c r="B35" s="313" t="n">
+        <v>-0.16</v>
+      </c>
+      <c r="C35" t="s">
+        <v>249</v>
+      </c>
+      <c r="D35" t="n" s="314">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>235</v>
+      </c>
+      <c r="B36" s="315" t="n">
+        <v>-0.24</v>
+      </c>
+      <c r="C36" t="s">
+        <v>249</v>
+      </c>
+      <c r="D36" t="n" s="316">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>237</v>
+      </c>
+      <c r="B37" s="317" t="n">
+        <v>-0.27</v>
+      </c>
+      <c r="C37" t="s">
+        <v>249</v>
+      </c>
+      <c r="D37" t="n" s="318">
+        <v>-0.03</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>239</v>
+      </c>
+      <c r="B38" s="319" t="n">
+        <v>-0.18</v>
+      </c>
+      <c r="C38" t="s">
+        <v>249</v>
+      </c>
+      <c r="D38" t="n" s="320">
+        <v>0.07</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>241</v>
+      </c>
+      <c r="B39" s="321" t="n">
+        <v>-0.57</v>
+      </c>
+      <c r="C39" t="s">
+        <v>249</v>
+      </c>
+      <c r="D39" t="n" s="322">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>243</v>
+      </c>
+      <c r="B40" s="323" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="C40" t="s">
+        <v>249</v>
+      </c>
+      <c r="D40" t="n" s="324">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" s="325" t="n">
+        <v>-0.15</v>
+      </c>
+      <c r="C41" t="n" s="326">
+        <v>-0.03</v>
+      </c>
+      <c r="D41" t="n" s="327">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>88</v>
+      </c>
+      <c r="B42" s="328" t="n">
+        <v>-0.32</v>
+      </c>
+      <c r="C42" t="n" s="329">
+        <v>-0.12</v>
+      </c>
+      <c r="D42" t="n" s="330">
+        <v>-0.08</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" s="331" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="C43" t="n" s="332">
+        <v>0.08</v>
+      </c>
+      <c r="D43" t="n" s="333">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>92</v>
+      </c>
+      <c r="B44" s="334" t="n">
+        <v>-0.21</v>
+      </c>
+      <c r="C44" t="n" s="335">
+        <v>-0.07</v>
+      </c>
+      <c r="D44" t="n" s="336">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>94</v>
+      </c>
+      <c r="B45" s="337" t="n">
+        <v>-0.32</v>
+      </c>
+      <c r="C45" t="n" s="338">
+        <v>-0.07</v>
+      </c>
+      <c r="D45" t="n" s="339">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>96</v>
+      </c>
+      <c r="B46" s="340" t="n">
+        <v>-0.08</v>
+      </c>
+      <c r="C46" t="n" s="341">
+        <v>-0.01</v>
+      </c>
+      <c r="D46" t="n" s="342">
+        <v>-0.03</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" s="343" t="n">
+        <v>-0.12</v>
+      </c>
+      <c r="C47" t="n" s="344">
+        <v>-0.01</v>
+      </c>
+      <c r="D47" t="n" s="345">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>100</v>
+      </c>
+      <c r="B48" s="346" t="n">
+        <v>-0.4</v>
+      </c>
+      <c r="C48" t="n" s="347">
+        <v>-0.09</v>
+      </c>
+      <c r="D48" t="n" s="348">
+        <v>-0.11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>102</v>
+      </c>
+      <c r="B49" s="349" t="n">
+        <v>-0.43</v>
+      </c>
+      <c r="C49" t="n" s="350">
+        <v>-0.11</v>
+      </c>
+      <c r="D49" t="n" s="351">
+        <v>-0.08</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>104</v>
+      </c>
+      <c r="B50" s="352" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="C50" t="n" s="353">
+        <v>0.0</v>
+      </c>
+      <c r="D50" t="n" s="354">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>106</v>
+      </c>
+      <c r="B51" s="355" t="n">
+        <v>-0.09</v>
+      </c>
+      <c r="C51" t="n" s="356">
+        <v>0.03</v>
+      </c>
+      <c r="D51" t="n" s="357">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" s="358" t="n">
+        <v>-0.14</v>
+      </c>
+      <c r="C52" t="n" s="359">
+        <v>-0.03</v>
+      </c>
+      <c r="D52" t="n" s="360">
+        <v>-0.07</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>109</v>
+      </c>
+      <c r="B53" s="361" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="C53" t="n" s="362">
+        <v>0.03</v>
+      </c>
+      <c r="D53" t="n" s="363">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>111</v>
+      </c>
+      <c r="B54" s="364" t="n">
+        <v>-0.34</v>
+      </c>
+      <c r="C54" t="n" s="365">
+        <v>-0.07</v>
+      </c>
+      <c r="D54" t="n" s="366">
+        <v>-0.09</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>113</v>
+      </c>
+      <c r="B55" s="367" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="C55" t="n" s="368">
+        <v>0.05</v>
+      </c>
+      <c r="D55" t="n" s="369">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>115</v>
+      </c>
+      <c r="B56" s="370" t="n">
+        <v>-0.08</v>
+      </c>
+      <c r="C56" t="n" s="371">
+        <v>0.01</v>
+      </c>
+      <c r="D56" t="n" s="372">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>117</v>
+      </c>
+      <c r="B57" s="373" t="n">
+        <v>-0.08</v>
+      </c>
+      <c r="C57" t="n" s="374">
+        <v>0.01</v>
+      </c>
+      <c r="D57" t="n" s="375">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>119</v>
+      </c>
+      <c r="B58" s="376" t="n">
+        <v>-0.07</v>
+      </c>
+      <c r="C58" t="n" s="377">
+        <v>0.04</v>
+      </c>
+      <c r="D58" t="n" s="378">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>121</v>
+      </c>
+      <c r="B59" s="379" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C59" t="n" s="380">
+        <v>0.06</v>
+      </c>
+      <c r="D59" t="n" s="381">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>123</v>
+      </c>
+      <c r="B60" s="382" t="n">
+        <v>-0.27</v>
+      </c>
+      <c r="C60" t="n" s="383">
+        <v>-0.05</v>
+      </c>
+      <c r="D60" t="n" s="384">
+        <v>-0.08</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>125</v>
+      </c>
+      <c r="B61" s="385" t="n">
+        <v>-0.42</v>
+      </c>
+      <c r="C61" t="n" s="386">
+        <v>0.0</v>
+      </c>
+      <c r="D61" t="n" s="387">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>127</v>
+      </c>
+      <c r="B62" s="388" t="n">
+        <v>-0.04</v>
+      </c>
+      <c r="C62" t="n" s="389">
+        <v>0.0</v>
+      </c>
+      <c r="D62" t="n" s="390">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>129</v>
+      </c>
+      <c r="B63" s="391" t="n">
+        <v>-0.12</v>
+      </c>
+      <c r="C63" t="n" s="392">
+        <v>-0.07</v>
+      </c>
+      <c r="D63" t="n" s="393">
+        <v>-0.07</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>131</v>
+      </c>
+      <c r="B64" s="394" t="n">
+        <v>-0.27</v>
+      </c>
+      <c r="C64" t="n" s="395">
+        <v>0.0</v>
+      </c>
+      <c r="D64" t="n" s="396">
+        <v>-0.07</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>133</v>
+      </c>
+      <c r="B65" s="397" t="n">
+        <v>-0.31</v>
+      </c>
+      <c r="C65" t="n" s="398">
+        <v>0.01</v>
+      </c>
+      <c r="D65" t="n" s="399">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>148</v>
+      </c>
+      <c r="B66" s="400" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="C66" t="n" s="401">
+        <v>0.17</v>
+      </c>
+      <c r="D66" t="n" s="402">
+        <v>0.04</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3924,10 +5262,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Init des indicateurs globaux
</commit_message>
<xml_diff>
--- a/src/main/resources/bourse.xlsx
+++ b/src/main/resources/bourse.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="254">
   <si>
     <t>AXA</t>
   </si>
@@ -779,6 +779,12 @@
   </si>
   <si>
     <t>% 2 days</t>
+  </si>
+  <si>
+    <t>20/04/2020</t>
+  </si>
+  <si>
+    <t>21/04/2020</t>
   </si>
 </sst>
 </file>
@@ -824,7 +830,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="403">
+  <cellXfs count="733">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -898,6 +904,336 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -4259,10 +4595,404 @@
       </c>
     </row>
     <row r="14" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
+      <c r="A14" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="B14" t="n">
+        <v>14.878</v>
+      </c>
+      <c r="C14" t="n">
+        <v>13.632</v>
+      </c>
+      <c r="D14" t="n">
+        <v>25.01</v>
+      </c>
+      <c r="E14" t="n">
+        <v>6.454</v>
+      </c>
+      <c r="F14" t="n">
+        <v>25.76</v>
+      </c>
+      <c r="G14" t="n">
+        <v>9.356</v>
+      </c>
+      <c r="H14" t="n">
+        <v>24.05</v>
+      </c>
+      <c r="I14" t="n">
+        <v>13.2</v>
+      </c>
+      <c r="J14" t="n">
+        <v>353.7</v>
+      </c>
+      <c r="K14" t="n">
+        <v>59.3</v>
+      </c>
+      <c r="L14" t="n">
+        <v>21.34</v>
+      </c>
+      <c r="M14" t="n">
+        <v>73.18</v>
+      </c>
+      <c r="N14" t="n">
+        <v>19.135</v>
+      </c>
+      <c r="O14" t="n">
+        <v>29.825</v>
+      </c>
+      <c r="P14" t="n">
+        <v>72.16</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>20.66</v>
+      </c>
+      <c r="R14" t="n">
+        <v>66.6</v>
+      </c>
+      <c r="S14" t="n">
+        <v>81.82</v>
+      </c>
+      <c r="T14" t="n">
+        <v>85.52</v>
+      </c>
+      <c r="U14" t="n">
+        <v>79.74</v>
+      </c>
+      <c r="V14" t="n">
+        <v>16.336</v>
+      </c>
+      <c r="W14" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="X14" t="n">
+        <v>87.3</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>11.275</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>139.4</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>11.63</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>14.01</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>63.04</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>136.7</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>110.8</v>
+      </c>
+      <c r="AF14" t="n">
+        <v>689.4</v>
+      </c>
+      <c r="AG14" t="n">
+        <v>501.4</v>
+      </c>
+      <c r="AH14" t="n">
+        <v>245.8</v>
+      </c>
+      <c r="AI14" t="n">
+        <v>59.2</v>
+      </c>
+      <c r="AJ14" t="n">
+        <v>80.92</v>
+      </c>
+      <c r="AK14" t="n">
+        <v>26.41</v>
+      </c>
+      <c r="AL14" t="n">
+        <v>63.6</v>
+      </c>
+      <c r="AM14" t="n">
+        <v>55.26</v>
+      </c>
+      <c r="AN14" t="n">
+        <v>119.55</v>
+      </c>
+      <c r="AO14" t="n">
+        <v>146.38</v>
+      </c>
+      <c r="AP14" t="n">
+        <v>87.38</v>
+      </c>
+      <c r="AQ14" t="n">
+        <v>282.8</v>
+      </c>
+      <c r="AR14" t="n">
+        <v>106.0</v>
+      </c>
+      <c r="AS14" t="n">
+        <v>87.2</v>
+      </c>
+      <c r="AT14" t="n">
+        <v>42.48</v>
+      </c>
+      <c r="AU14" t="n">
+        <v>48.07</v>
+      </c>
+      <c r="AV14" t="n">
+        <v>33.41</v>
+      </c>
+      <c r="AW14" t="n">
+        <v>43.21</v>
+      </c>
+      <c r="AX14" t="n">
+        <v>183.41</v>
+      </c>
+      <c r="AY14" t="n">
+        <v>209.4</v>
+      </c>
+      <c r="AZ14" t="n">
+        <v>120.11</v>
+      </c>
+      <c r="BA14" t="n">
+        <v>60.36</v>
+      </c>
+      <c r="BB14" t="n">
+        <v>95.0</v>
+      </c>
+      <c r="BC14" t="n">
+        <v>151.92</v>
+      </c>
+      <c r="BD14" t="n">
+        <v>186.1</v>
+      </c>
+      <c r="BE14" t="n">
+        <v>89.87</v>
+      </c>
+      <c r="BF14" t="n">
+        <v>36.9</v>
+      </c>
+      <c r="BG14" t="n">
+        <v>124.66</v>
+      </c>
+      <c r="BH14" t="n">
+        <v>105.1</v>
+      </c>
+      <c r="BI14" t="n">
+        <v>86.14</v>
+      </c>
+      <c r="BJ14" t="n">
+        <v>58.47</v>
+      </c>
+      <c r="BK14" t="n">
+        <v>169.37</v>
+      </c>
+      <c r="BL14" t="n">
+        <v>44.5</v>
+      </c>
+      <c r="BM14" t="n">
+        <v>106.65</v>
+      </c>
+      <c r="BN14" t="n">
+        <v>56.6</v>
+      </c>
     </row>
     <row r="15" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
+      <c r="A15" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="B15" t="n">
+        <v>14.668</v>
+      </c>
+      <c r="C15" t="n">
+        <v>13.43</v>
+      </c>
+      <c r="D15" t="n">
+        <v>24.85</v>
+      </c>
+      <c r="E15" t="n">
+        <v>6.364</v>
+      </c>
+      <c r="F15" t="n">
+        <v>26.26</v>
+      </c>
+      <c r="G15" t="n">
+        <v>9.21</v>
+      </c>
+      <c r="H15" t="n">
+        <v>23.94</v>
+      </c>
+      <c r="I15" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>354.45</v>
+      </c>
+      <c r="K15" t="n">
+        <v>59.64</v>
+      </c>
+      <c r="L15" t="n">
+        <v>20.69</v>
+      </c>
+      <c r="M15" t="n">
+        <v>72.28</v>
+      </c>
+      <c r="N15" t="n">
+        <v>17.785</v>
+      </c>
+      <c r="O15" t="n">
+        <v>29.48</v>
+      </c>
+      <c r="P15" t="n">
+        <v>71.46</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>20.58</v>
+      </c>
+      <c r="R15" t="n">
+        <v>66.9</v>
+      </c>
+      <c r="S15" t="n">
+        <v>82.38</v>
+      </c>
+      <c r="T15" t="n">
+        <v>88.39</v>
+      </c>
+      <c r="U15" t="n">
+        <v>76.88</v>
+      </c>
+      <c r="V15" t="n">
+        <v>16.222</v>
+      </c>
+      <c r="W15" t="n">
+        <v>25.23</v>
+      </c>
+      <c r="X15" t="n">
+        <v>86.82</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>11.18</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>139.0</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>11.68</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>13.855</v>
+      </c>
+      <c r="AC15" t="n">
+        <v>63.24</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>135.1</v>
+      </c>
+      <c r="AE15" t="n">
+        <v>108.0</v>
+      </c>
+      <c r="AF15" t="n">
+        <v>684.6</v>
+      </c>
+      <c r="AG15" t="n">
+        <v>497.8</v>
+      </c>
+      <c r="AH15" t="n">
+        <v>254.8</v>
+      </c>
+      <c r="AI15" t="n">
+        <v>55.96</v>
+      </c>
+      <c r="AJ15" t="n">
+        <v>80.54</v>
+      </c>
+      <c r="AK15" t="n">
+        <v>25.59</v>
+      </c>
+      <c r="AL15" t="n">
+        <v>64.78</v>
+      </c>
+      <c r="AM15" t="n">
+        <v>53.02</v>
+      </c>
+      <c r="AN15" t="n">
+        <v>119.4</v>
+      </c>
+      <c r="AO15" t="n">
+        <v>143.7</v>
+      </c>
+      <c r="AP15" t="n">
+        <v>84.01</v>
+      </c>
+      <c r="AQ15" t="n">
+        <v>276.93</v>
+      </c>
+      <c r="AR15" t="n">
+        <v>106.5</v>
+      </c>
+      <c r="AS15" t="n">
+        <v>83.51</v>
+      </c>
+      <c r="AT15" t="n">
+        <v>42.54</v>
+      </c>
+      <c r="AU15" t="n">
+        <v>46.59</v>
+      </c>
+      <c r="AV15" t="n">
+        <v>31.53</v>
+      </c>
+      <c r="AW15" t="n">
+        <v>41.18</v>
+      </c>
+      <c r="AX15" t="n">
+        <v>180.5</v>
+      </c>
+      <c r="AY15" t="n">
+        <v>206.16</v>
+      </c>
+      <c r="AZ15" t="n">
+        <v>120.58</v>
+      </c>
+      <c r="BA15" t="n">
+        <v>59.18</v>
+      </c>
+      <c r="BB15" t="n">
+        <v>91.64</v>
+      </c>
+      <c r="BC15" t="n">
+        <v>151.83</v>
+      </c>
+      <c r="BD15" t="n">
+        <v>181.7</v>
+      </c>
+      <c r="BE15" t="n">
+        <v>87.86</v>
+      </c>
+      <c r="BF15" t="n">
+        <v>36.08</v>
+      </c>
+      <c r="BG15" t="n">
+        <v>120.58</v>
+      </c>
+      <c r="BH15" t="n">
+        <v>101.75</v>
+      </c>
+      <c r="BI15" t="n">
+        <v>86.14</v>
+      </c>
+      <c r="BJ15" t="n">
+        <v>58.15</v>
+      </c>
+      <c r="BK15" t="n">
+        <v>164.22</v>
+      </c>
+      <c r="BL15" t="n">
+        <v>42.85</v>
+      </c>
+      <c r="BM15" t="n">
+        <v>102.21</v>
+      </c>
+      <c r="BN15" t="n">
+        <v>56.97</v>
+      </c>
     </row>
     <row r="16" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
@@ -4346,139 +5076,139 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="238" t="n">
-        <v>-0.39</v>
-      </c>
-      <c r="C2" t="n" s="239">
+      <c r="B2" s="568" t="n">
+        <v>-0.41</v>
+      </c>
+      <c r="C2" t="n" s="569">
+        <v>-0.06</v>
+      </c>
+      <c r="D2" t="n" s="570">
         <v>-0.02</v>
-      </c>
-      <c r="D2" t="n" s="240">
-        <v>0.0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="241" t="n">
-        <v>-0.51</v>
-      </c>
-      <c r="C3" t="n" s="242">
-        <v>-0.05</v>
-      </c>
-      <c r="D3" t="n" s="243">
-        <v>0.01</v>
+      <c r="B3" s="571" t="n">
+        <v>-0.53</v>
+      </c>
+      <c r="C3" t="n" s="572">
+        <v>-0.11</v>
+      </c>
+      <c r="D3" t="n" s="573">
+        <v>-0.04</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="244" t="n">
-        <v>-0.49</v>
-      </c>
-      <c r="C4" t="n" s="245">
-        <v>-0.07</v>
-      </c>
-      <c r="D4" t="n" s="246">
-        <v>-0.02</v>
+      <c r="B4" s="574" t="n">
+        <v>-0.51</v>
+      </c>
+      <c r="C4" t="n" s="575">
+        <v>-0.12</v>
+      </c>
+      <c r="D4" t="n" s="576">
+        <v>-0.05</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="247" t="n">
-        <v>-0.48</v>
-      </c>
-      <c r="C5" t="n" s="248">
-        <v>-0.05</v>
-      </c>
-      <c r="D5" t="n" s="249">
-        <v>0.01</v>
+      <c r="B5" s="577" t="n">
+        <v>-0.49</v>
+      </c>
+      <c r="C5" t="n" s="578">
+        <v>-0.07</v>
+      </c>
+      <c r="D5" t="n" s="579">
+        <v>-0.02</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>78</v>
       </c>
-      <c r="B6" s="250" t="n">
-        <v>-0.33</v>
-      </c>
-      <c r="C6" t="n" s="251">
-        <v>-0.08</v>
-      </c>
-      <c r="D6" t="n" s="252">
-        <v>0.02</v>
+      <c r="B6" s="580" t="n">
+        <v>-0.32</v>
+      </c>
+      <c r="C6" t="n" s="581">
+        <v>-0.06</v>
+      </c>
+      <c r="D6" t="n" s="582">
+        <v>0.0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="253" t="n">
-        <v>-0.34</v>
-      </c>
-      <c r="C7" t="n" s="254">
-        <v>-0.01</v>
-      </c>
-      <c r="D7" t="n" s="255">
-        <v>0.0</v>
+      <c r="B7" s="583" t="n">
+        <v>-0.36</v>
+      </c>
+      <c r="C7" t="n" s="584">
+        <v>-0.06</v>
+      </c>
+      <c r="D7" t="n" s="585">
+        <v>-0.04</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="256" t="n">
-        <v>-0.32</v>
-      </c>
-      <c r="C8" t="n" s="257">
-        <v>-0.03</v>
-      </c>
-      <c r="D8" t="n" s="258">
-        <v>0.04</v>
+      <c r="B8" s="586" t="n">
+        <v>-0.35</v>
+      </c>
+      <c r="C8" t="n" s="587">
+        <v>-0.06</v>
+      </c>
+      <c r="D8" t="n" s="588">
+        <v>-0.04</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>84</v>
       </c>
-      <c r="B9" s="259" t="n">
-        <v>-0.58</v>
-      </c>
-      <c r="C9" t="n" s="260">
-        <v>-0.15</v>
-      </c>
-      <c r="D9" t="n" s="261">
-        <v>0.0</v>
+      <c r="B9" s="589" t="n">
+        <v>-0.61</v>
+      </c>
+      <c r="C9" t="n" s="590">
+        <v>-0.13</v>
+      </c>
+      <c r="D9" t="n" s="591">
+        <v>-0.07</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>150</v>
       </c>
-      <c r="B10" s="262" t="n">
-        <v>-0.12</v>
-      </c>
-      <c r="C10" t="n" s="263">
-        <v>0.06</v>
-      </c>
-      <c r="D10" t="n" s="264">
-        <v>0.04</v>
+      <c r="B10" s="592" t="n">
+        <v>-0.13</v>
+      </c>
+      <c r="C10" t="n" s="593">
+        <v>0.0</v>
+      </c>
+      <c r="D10" t="n" s="594">
+        <v>-0.02</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>185</v>
       </c>
-      <c r="B11" s="265" t="n">
-        <v>0.0</v>
+      <c r="B11" s="595" t="n">
+        <v>0.01</v>
       </c>
       <c r="C11" t="s">
         <v>249</v>
       </c>
-      <c r="D11" t="n" s="266">
+      <c r="D11" t="n" s="596">
         <v>0.01</v>
       </c>
     </row>
@@ -4486,125 +5216,125 @@
       <c r="A12" t="s">
         <v>187</v>
       </c>
-      <c r="B12" s="267" t="n">
-        <v>-0.19</v>
+      <c r="B12" s="597" t="n">
+        <v>-0.17</v>
       </c>
       <c r="C12" t="s">
         <v>249</v>
       </c>
-      <c r="D12" t="n" s="268">
-        <v>-0.02</v>
+      <c r="D12" t="n" s="598">
+        <v>0.02</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>189</v>
       </c>
-      <c r="B13" s="269" t="n">
-        <v>-0.22</v>
+      <c r="B13" s="599" t="n">
+        <v>-0.27</v>
       </c>
       <c r="C13" t="s">
         <v>249</v>
       </c>
-      <c r="D13" t="n" s="270">
-        <v>0.04</v>
+      <c r="D13" t="n" s="600">
+        <v>-0.06</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>191</v>
       </c>
-      <c r="B14" s="271" t="n">
-        <v>-0.13</v>
+      <c r="B14" s="601" t="n">
+        <v>-0.24</v>
       </c>
       <c r="C14" t="s">
         <v>249</v>
       </c>
-      <c r="D14" t="n" s="272">
-        <v>0.07</v>
+      <c r="D14" t="n" s="602">
+        <v>-0.12</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>193</v>
       </c>
-      <c r="B15" s="273" t="n">
-        <v>-0.34</v>
+      <c r="B15" s="603" t="n">
+        <v>-0.38</v>
       </c>
       <c r="C15" t="s">
         <v>249</v>
       </c>
-      <c r="D15" t="n" s="274">
-        <v>0.02</v>
+      <c r="D15" t="n" s="604">
+        <v>-0.06</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>195</v>
       </c>
-      <c r="B16" s="275" t="n">
-        <v>-0.18</v>
+      <c r="B16" s="605" t="n">
+        <v>-0.2</v>
       </c>
       <c r="C16" t="s">
         <v>249</v>
       </c>
-      <c r="D16" t="n" s="276">
-        <v>0.04</v>
+      <c r="D16" t="n" s="606">
+        <v>-0.02</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>197</v>
       </c>
-      <c r="B17" s="277" t="n">
-        <v>-0.04</v>
+      <c r="B17" s="607" t="n">
+        <v>-0.08</v>
       </c>
       <c r="C17" t="s">
         <v>249</v>
       </c>
-      <c r="D17" t="n" s="278">
-        <v>0.02</v>
+      <c r="D17" t="n" s="608">
+        <v>-0.04</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>199</v>
       </c>
-      <c r="B18" s="279" t="n">
-        <v>-0.39</v>
+      <c r="B18" s="609" t="n">
+        <v>-0.37</v>
       </c>
       <c r="C18" t="s">
         <v>249</v>
       </c>
-      <c r="D18" t="n" s="280">
-        <v>-0.02</v>
+      <c r="D18" t="n" s="610">
+        <v>0.03</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>201</v>
       </c>
-      <c r="B19" s="281" t="n">
-        <v>-0.04</v>
+      <c r="B19" s="611" t="n">
+        <v>-0.06</v>
       </c>
       <c r="C19" t="s">
         <v>249</v>
       </c>
-      <c r="D19" t="n" s="282">
-        <v>0.04</v>
+      <c r="D19" t="n" s="612">
+        <v>-0.02</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>203</v>
       </c>
-      <c r="B20" s="283" t="n">
-        <v>0.02</v>
+      <c r="B20" s="613" t="n">
+        <v>0.04</v>
       </c>
       <c r="C20" t="s">
         <v>249</v>
       </c>
-      <c r="D20" t="n" s="284">
+      <c r="D20" t="n" s="614">
         <v>0.02</v>
       </c>
     </row>
@@ -4612,335 +5342,335 @@
       <c r="A21" t="s">
         <v>205</v>
       </c>
-      <c r="B21" s="285" t="n">
-        <v>-0.45</v>
+      <c r="B21" s="615" t="n">
+        <v>-0.48</v>
       </c>
       <c r="C21" t="s">
         <v>249</v>
       </c>
-      <c r="D21" t="n" s="286">
-        <v>0.08</v>
+      <c r="D21" t="n" s="616">
+        <v>-0.06</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>207</v>
       </c>
-      <c r="B22" s="287" t="n">
-        <v>-0.62</v>
+      <c r="B22" s="617" t="n">
+        <v>-0.63</v>
       </c>
       <c r="C22" t="s">
         <v>249</v>
       </c>
-      <c r="D22" t="n" s="288">
-        <v>-0.03</v>
+      <c r="D22" t="n" s="618">
+        <v>-0.02</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>209</v>
       </c>
-      <c r="B23" s="289" t="n">
-        <v>-0.34</v>
+      <c r="B23" s="619" t="n">
+        <v>-0.37</v>
       </c>
       <c r="C23" t="s">
         <v>249</v>
       </c>
-      <c r="D23" t="n" s="290">
-        <v>-0.08</v>
+      <c r="D23" t="n" s="620">
+        <v>-0.04</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>211</v>
       </c>
-      <c r="B24" s="291" t="n">
-        <v>-0.18</v>
+      <c r="B24" s="621" t="n">
+        <v>-0.2</v>
       </c>
       <c r="C24" t="s">
         <v>249</v>
       </c>
-      <c r="D24" t="n" s="292">
-        <v>0.06</v>
+      <c r="D24" t="n" s="622">
+        <v>-0.03</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>213</v>
       </c>
-      <c r="B25" s="293" t="n">
-        <v>-0.23</v>
+      <c r="B25" s="623" t="n">
+        <v>-0.24</v>
       </c>
       <c r="C25" t="s">
         <v>249</v>
       </c>
-      <c r="D25" t="n" s="294">
-        <v>0.0</v>
+      <c r="D25" t="n" s="624">
+        <v>-0.02</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>215</v>
       </c>
-      <c r="B26" s="295" t="n">
+      <c r="B26" s="625" t="n">
         <v>-0.16</v>
       </c>
       <c r="C26" t="s">
         <v>249</v>
       </c>
-      <c r="D26" t="n" s="296">
-        <v>0.01</v>
+      <c r="D26" t="n" s="626">
+        <v>-0.01</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>217</v>
       </c>
-      <c r="B27" s="297" t="n">
+      <c r="B27" s="627" t="n">
         <v>-0.47</v>
       </c>
       <c r="C27" t="s">
         <v>249</v>
       </c>
-      <c r="D27" t="n" s="298">
-        <v>-0.05</v>
+      <c r="D27" t="n" s="628">
+        <v>0.01</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>219</v>
       </c>
-      <c r="B28" s="299" t="n">
-        <v>-0.07</v>
+      <c r="B28" s="629" t="n">
+        <v>-0.08</v>
       </c>
       <c r="C28" t="s">
         <v>249</v>
       </c>
-      <c r="D28" t="n" s="300">
-        <v>-0.02</v>
+      <c r="D28" t="n" s="630">
+        <v>0.0</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>221</v>
       </c>
-      <c r="B29" s="301" t="n">
+      <c r="B29" s="631" t="n">
         <v>-0.15</v>
       </c>
       <c r="C29" t="s">
         <v>249</v>
       </c>
-      <c r="D29" t="n" s="302">
-        <v>0.03</v>
+      <c r="D29" t="n" s="632">
+        <v>-0.01</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>223</v>
       </c>
-      <c r="B30" s="303" t="n">
-        <v>-0.02</v>
+      <c r="B30" s="633" t="n">
+        <v>-0.06</v>
       </c>
       <c r="C30" t="s">
         <v>249</v>
       </c>
-      <c r="D30" t="n" s="304">
-        <v>0.05</v>
+      <c r="D30" t="n" s="634">
+        <v>-0.04</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>225</v>
       </c>
-      <c r="B31" s="305" t="n">
+      <c r="B31" s="635" t="n">
         <v>-0.23</v>
       </c>
       <c r="C31" t="s">
         <v>249</v>
       </c>
-      <c r="D31" t="n" s="306">
-        <v>0.02</v>
+      <c r="D31" t="n" s="636">
+        <v>0.0</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>227</v>
       </c>
-      <c r="B32" s="307" t="n">
-        <v>0.01</v>
+      <c r="B32" s="637" t="n">
+        <v>0.0</v>
       </c>
       <c r="C32" t="s">
         <v>249</v>
       </c>
-      <c r="D32" t="n" s="308">
-        <v>0.02</v>
+      <c r="D32" t="n" s="638">
+        <v>0.0</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>229</v>
       </c>
-      <c r="B33" s="309" t="n">
-        <v>-0.07</v>
+      <c r="B33" s="639" t="n">
+        <v>-0.09</v>
       </c>
       <c r="C33" t="s">
         <v>249</v>
       </c>
-      <c r="D33" t="n" s="310">
-        <v>0.06</v>
+      <c r="D33" t="n" s="640">
+        <v>-0.02</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>231</v>
       </c>
-      <c r="B34" s="311" t="n">
-        <v>-0.03</v>
+      <c r="B34" s="641" t="n">
+        <v>-0.01</v>
       </c>
       <c r="C34" t="s">
         <v>249</v>
       </c>
-      <c r="D34" t="n" s="312">
-        <v>-0.01</v>
+      <c r="D34" t="n" s="642">
+        <v>0.02</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>233</v>
       </c>
-      <c r="B35" s="313" t="n">
-        <v>-0.16</v>
+      <c r="B35" s="643" t="n">
+        <v>-0.22</v>
       </c>
       <c r="C35" t="s">
         <v>249</v>
       </c>
-      <c r="D35" t="n" s="314">
-        <v>0.02</v>
+      <c r="D35" t="n" s="644">
+        <v>-0.07</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>235</v>
       </c>
-      <c r="B36" s="315" t="n">
-        <v>-0.24</v>
+      <c r="B36" s="645" t="n">
+        <v>-0.25</v>
       </c>
       <c r="C36" t="s">
         <v>249</v>
       </c>
-      <c r="D36" t="n" s="316">
-        <v>0.02</v>
+      <c r="D36" t="n" s="646">
+        <v>-0.02</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>237</v>
       </c>
-      <c r="B37" s="317" t="n">
-        <v>-0.27</v>
+      <c r="B37" s="647" t="n">
+        <v>-0.31</v>
       </c>
       <c r="C37" t="s">
         <v>249</v>
       </c>
-      <c r="D37" t="n" s="318">
-        <v>-0.03</v>
+      <c r="D37" t="n" s="648">
+        <v>-0.05</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>239</v>
       </c>
-      <c r="B38" s="319" t="n">
-        <v>-0.18</v>
+      <c r="B38" s="649" t="n">
+        <v>-0.16</v>
       </c>
       <c r="C38" t="s">
         <v>249</v>
       </c>
-      <c r="D38" t="n" s="320">
-        <v>0.07</v>
+      <c r="D38" t="n" s="650">
+        <v>0.02</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>241</v>
       </c>
-      <c r="B39" s="321" t="n">
-        <v>-0.57</v>
+      <c r="B39" s="651" t="n">
+        <v>-0.6</v>
       </c>
       <c r="C39" t="s">
         <v>249</v>
       </c>
-      <c r="D39" t="n" s="322">
-        <v>0.01</v>
+      <c r="D39" t="n" s="652">
+        <v>-0.08</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>243</v>
       </c>
-      <c r="B40" s="323" t="n">
-        <v>-0.01</v>
+      <c r="B40" s="653" t="n">
+        <v>-0.03</v>
       </c>
       <c r="C40" t="s">
         <v>249</v>
       </c>
-      <c r="D40" t="n" s="324">
-        <v>-0.02</v>
+      <c r="D40" t="n" s="654">
+        <v>-0.01</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>86</v>
       </c>
-      <c r="B41" s="325" t="n">
-        <v>-0.15</v>
-      </c>
-      <c r="C41" t="n" s="326">
-        <v>-0.03</v>
-      </c>
-      <c r="D41" t="n" s="327">
-        <v>-0.04</v>
+      <c r="B41" s="655" t="n">
+        <v>-0.16</v>
+      </c>
+      <c r="C41" t="n" s="656">
+        <v>-0.02</v>
+      </c>
+      <c r="D41" t="n" s="657">
+        <v>-0.01</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>88</v>
       </c>
-      <c r="B42" s="328" t="n">
-        <v>-0.32</v>
-      </c>
-      <c r="C42" t="n" s="329">
-        <v>-0.12</v>
-      </c>
-      <c r="D42" t="n" s="330">
-        <v>-0.08</v>
+      <c r="B42" s="658" t="n">
+        <v>-0.3</v>
+      </c>
+      <c r="C42" t="n" s="659">
+        <v>-0.07</v>
+      </c>
+      <c r="D42" t="n" s="660">
+        <v>0.03</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>90</v>
       </c>
-      <c r="B43" s="331" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="C43" t="n" s="332">
-        <v>0.08</v>
-      </c>
-      <c r="D43" t="n" s="333">
-        <v>0.0</v>
+      <c r="B43" s="661" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="C43" t="n" s="662">
+        <v>-0.01</v>
+      </c>
+      <c r="D43" t="n" s="663">
+        <v>-0.03</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>92</v>
       </c>
-      <c r="B44" s="334" t="n">
-        <v>-0.21</v>
-      </c>
-      <c r="C44" t="n" s="335">
+      <c r="B44" s="664" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="C44" t="n" s="665">
         <v>-0.07</v>
       </c>
-      <c r="D44" t="n" s="336">
+      <c r="D44" t="n" s="666">
         <v>0.0</v>
       </c>
     </row>
@@ -4948,237 +5678,237 @@
       <c r="A45" t="s">
         <v>94</v>
       </c>
-      <c r="B45" s="337" t="n">
-        <v>-0.32</v>
-      </c>
-      <c r="C45" t="n" s="338">
-        <v>-0.07</v>
-      </c>
-      <c r="D45" t="n" s="339">
-        <v>-0.05</v>
+      <c r="B45" s="667" t="n">
+        <v>-0.29</v>
+      </c>
+      <c r="C45" t="n" s="668">
+        <v>-0.02</v>
+      </c>
+      <c r="D45" t="n" s="669">
+        <v>0.04</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>96</v>
       </c>
-      <c r="B46" s="340" t="n">
-        <v>-0.08</v>
-      </c>
-      <c r="C46" t="n" s="341">
-        <v>-0.01</v>
-      </c>
-      <c r="D46" t="n" s="342">
-        <v>-0.03</v>
+      <c r="B46" s="670" t="n">
+        <v>-0.06</v>
+      </c>
+      <c r="C46" t="n" s="671">
+        <v>0.03</v>
+      </c>
+      <c r="D46" t="n" s="672">
+        <v>0.03</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>98</v>
       </c>
-      <c r="B47" s="343" t="n">
-        <v>-0.12</v>
-      </c>
-      <c r="C47" t="n" s="344">
+      <c r="B47" s="673" t="n">
+        <v>-0.13</v>
+      </c>
+      <c r="C47" t="n" s="674">
         <v>-0.01</v>
       </c>
-      <c r="D47" t="n" s="345">
-        <v>-0.04</v>
+      <c r="D47" t="n" s="675">
+        <v>-0.01</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>100</v>
       </c>
-      <c r="B48" s="346" t="n">
-        <v>-0.4</v>
-      </c>
-      <c r="C48" t="n" s="347">
-        <v>-0.09</v>
-      </c>
-      <c r="D48" t="n" s="348">
-        <v>-0.11</v>
+      <c r="B48" s="676" t="n">
+        <v>-0.41</v>
+      </c>
+      <c r="C48" t="n" s="677">
+        <v>-0.1</v>
+      </c>
+      <c r="D48" t="n" s="678">
+        <v>0.0</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>102</v>
       </c>
-      <c r="B49" s="349" t="n">
-        <v>-0.43</v>
-      </c>
-      <c r="C49" t="n" s="350">
-        <v>-0.11</v>
-      </c>
-      <c r="D49" t="n" s="351">
-        <v>-0.08</v>
+      <c r="B49" s="679" t="n">
+        <v>-0.4</v>
+      </c>
+      <c r="C49" t="n" s="680">
+        <v>-0.04</v>
+      </c>
+      <c r="D49" t="n" s="681">
+        <v>0.05</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>104</v>
       </c>
-      <c r="B50" s="352" t="n">
-        <v>-0.2</v>
-      </c>
-      <c r="C50" t="n" s="353">
-        <v>0.0</v>
-      </c>
-      <c r="D50" t="n" s="354">
-        <v>-0.01</v>
+      <c r="B50" s="682" t="n">
+        <v>-0.18</v>
+      </c>
+      <c r="C50" t="n" s="683">
+        <v>0.01</v>
+      </c>
+      <c r="D50" t="n" s="684">
+        <v>0.02</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>106</v>
       </c>
-      <c r="B51" s="355" t="n">
-        <v>-0.09</v>
-      </c>
-      <c r="C51" t="n" s="356">
+      <c r="B51" s="685" t="n">
+        <v>-0.07</v>
+      </c>
+      <c r="C51" t="n" s="686">
+        <v>0.04</v>
+      </c>
+      <c r="D51" t="n" s="687">
         <v>0.03</v>
-      </c>
-      <c r="D51" t="n" s="357">
-        <v>-0.04</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>10</v>
       </c>
-      <c r="B52" s="358" t="n">
-        <v>-0.14</v>
-      </c>
-      <c r="C52" t="n" s="359">
-        <v>-0.03</v>
-      </c>
-      <c r="D52" t="n" s="360">
-        <v>-0.07</v>
+      <c r="B52" s="688" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="C52" t="n" s="689">
+        <v>-0.01</v>
+      </c>
+      <c r="D52" t="n" s="690">
+        <v>0.04</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>109</v>
       </c>
-      <c r="B53" s="361" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="C53" t="n" s="362">
-        <v>0.03</v>
-      </c>
-      <c r="D53" t="n" s="363">
-        <v>0.0</v>
+      <c r="B53" s="691" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C53" t="n" s="692">
+        <v>0.01</v>
+      </c>
+      <c r="D53" t="n" s="693">
+        <v>-0.03</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>111</v>
       </c>
-      <c r="B54" s="364" t="n">
-        <v>-0.34</v>
-      </c>
-      <c r="C54" t="n" s="365">
+      <c r="B54" s="694" t="n">
+        <v>-0.31</v>
+      </c>
+      <c r="C54" t="n" s="695">
         <v>-0.07</v>
       </c>
-      <c r="D54" t="n" s="366">
-        <v>-0.09</v>
+      <c r="D54" t="n" s="696">
+        <v>0.05</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>113</v>
       </c>
-      <c r="B55" s="367" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="C55" t="n" s="368">
-        <v>0.05</v>
-      </c>
-      <c r="D55" t="n" s="369">
-        <v>0.03</v>
+      <c r="B55" s="697" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C55" t="n" s="698">
+        <v>0.08</v>
+      </c>
+      <c r="D55" t="n" s="699">
+        <v>0.01</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>115</v>
       </c>
-      <c r="B56" s="370" t="n">
-        <v>-0.08</v>
-      </c>
-      <c r="C56" t="n" s="371">
+      <c r="B56" s="700" t="n">
+        <v>-0.07</v>
+      </c>
+      <c r="C56" t="n" s="701">
         <v>0.01</v>
       </c>
-      <c r="D56" t="n" s="372">
-        <v>-0.02</v>
+      <c r="D56" t="n" s="702">
+        <v>0.01</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>117</v>
       </c>
-      <c r="B57" s="373" t="n">
-        <v>-0.08</v>
-      </c>
-      <c r="C57" t="n" s="374">
-        <v>0.01</v>
-      </c>
-      <c r="D57" t="n" s="375">
-        <v>-0.01</v>
+      <c r="B57" s="703" t="n">
+        <v>-0.07</v>
+      </c>
+      <c r="C57" t="n" s="704">
+        <v>0.04</v>
+      </c>
+      <c r="D57" t="n" s="705">
+        <v>0.02</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>119</v>
       </c>
-      <c r="B58" s="376" t="n">
+      <c r="B58" s="706" t="n">
         <v>-0.07</v>
       </c>
-      <c r="C58" t="n" s="377">
-        <v>0.04</v>
-      </c>
-      <c r="D58" t="n" s="378">
-        <v>-0.01</v>
+      <c r="C58" t="n" s="707">
+        <v>0.03</v>
+      </c>
+      <c r="D58" t="n" s="708">
+        <v>0.0</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>121</v>
       </c>
-      <c r="B59" s="379" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="C59" t="n" s="380">
-        <v>0.06</v>
-      </c>
-      <c r="D59" t="n" s="381">
-        <v>0.0</v>
+      <c r="B59" s="709" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="C59" t="n" s="710">
+        <v>0.04</v>
+      </c>
+      <c r="D59" t="n" s="711">
+        <v>-0.01</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>123</v>
       </c>
-      <c r="B60" s="382" t="n">
-        <v>-0.27</v>
-      </c>
-      <c r="C60" t="n" s="383">
-        <v>-0.05</v>
-      </c>
-      <c r="D60" t="n" s="384">
-        <v>-0.08</v>
+      <c r="B60" s="712" t="n">
+        <v>-0.26</v>
+      </c>
+      <c r="C60" t="n" s="713">
+        <v>-0.04</v>
+      </c>
+      <c r="D60" t="n" s="714">
+        <v>0.02</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>125</v>
       </c>
-      <c r="B61" s="385" t="n">
+      <c r="B61" s="715" t="n">
         <v>-0.42</v>
       </c>
-      <c r="C61" t="n" s="386">
+      <c r="C61" t="n" s="716">
         <v>0.0</v>
       </c>
-      <c r="D61" t="n" s="387">
+      <c r="D61" t="n" s="717">
         <v>0.0</v>
       </c>
     </row>
@@ -5186,70 +5916,70 @@
       <c r="A62" t="s">
         <v>127</v>
       </c>
-      <c r="B62" s="388" t="n">
-        <v>-0.04</v>
-      </c>
-      <c r="C62" t="n" s="389">
-        <v>0.0</v>
-      </c>
-      <c r="D62" t="n" s="390">
-        <v>-0.01</v>
+      <c r="B62" s="718" t="n">
+        <v>-0.03</v>
+      </c>
+      <c r="C62" t="n" s="719">
+        <v>0.03</v>
+      </c>
+      <c r="D62" t="n" s="720">
+        <v>0.01</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>129</v>
       </c>
-      <c r="B63" s="391" t="n">
-        <v>-0.12</v>
-      </c>
-      <c r="C63" t="n" s="392">
-        <v>-0.07</v>
-      </c>
-      <c r="D63" t="n" s="393">
-        <v>-0.07</v>
+      <c r="B63" s="721" t="n">
+        <v>-0.11</v>
+      </c>
+      <c r="C63" t="n" s="722">
+        <v>-0.03</v>
+      </c>
+      <c r="D63" t="n" s="723">
+        <v>0.01</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>131</v>
       </c>
-      <c r="B64" s="394" t="n">
-        <v>-0.27</v>
-      </c>
-      <c r="C64" t="n" s="395">
-        <v>0.0</v>
-      </c>
-      <c r="D64" t="n" s="396">
-        <v>-0.07</v>
+      <c r="B64" s="724" t="n">
+        <v>-0.28</v>
+      </c>
+      <c r="C64" t="n" s="725">
+        <v>-0.05</v>
+      </c>
+      <c r="D64" t="n" s="726">
+        <v>-0.01</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>133</v>
       </c>
-      <c r="B65" s="397" t="n">
-        <v>-0.31</v>
-      </c>
-      <c r="C65" t="n" s="398">
-        <v>0.01</v>
-      </c>
-      <c r="D65" t="n" s="399">
-        <v>-0.04</v>
+      <c r="B65" s="727" t="n">
+        <v>-0.3</v>
+      </c>
+      <c r="C65" t="n" s="728">
+        <v>-0.01</v>
+      </c>
+      <c r="D65" t="n" s="729">
+        <v>0.0</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>148</v>
       </c>
-      <c r="B66" s="400" t="n">
+      <c r="B66" s="730" t="n">
         <v>0.45</v>
       </c>
-      <c r="C66" t="n" s="401">
-        <v>0.17</v>
-      </c>
-      <c r="D66" t="n" s="402">
-        <v>0.04</v>
+      <c r="C66" t="n" s="731">
+        <v>0.09</v>
+      </c>
+      <c r="D66" t="n" s="732">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout indicateurs globaux et feuille de synthese
</commit_message>
<xml_diff>
--- a/src/main/resources/bourse.xlsx
+++ b/src/main/resources/bourse.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="13995" windowHeight="5610" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="13995" windowHeight="5610" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="282">
   <si>
     <t>AXA</t>
   </si>
@@ -766,9 +766,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>diff from ref (%)</t>
-  </si>
-  <si>
     <t>% ref</t>
   </si>
   <si>
@@ -785,6 +782,93 @@
   </si>
   <si>
     <t>21/04/2020</t>
+  </si>
+  <si>
+    <t>% moyen ref (65.0)</t>
+  </si>
+  <si>
+    <t>Pourcentage moyen entre le cours actuel et le cours de ref (Ex : -40% si le cours est passé de 10 (ref) à 6 (actuel))</t>
+  </si>
+  <si>
+    <t>% moyen baissier ref (58.0)</t>
+  </si>
+  <si>
+    <t>Pourcentage moyen des actions baissieres entre le cours actuel et le cours de ref (Ex : -40% si le cours est passé de 10 (ref) à 6 (actuel))</t>
+  </si>
+  <si>
+    <t>Pourcentage moyen entre le cours actuel et le cours d'il y a une semaine (Ex : -10% si le cours est passé de 10 (il y a une semaine) à 9 (actuel))</t>
+  </si>
+  <si>
+    <t>% Top 10 baissier ref (10)</t>
+  </si>
+  <si>
+    <t>Top 10 des actions ayant le plus baissé depuis le cours de référence</t>
+  </si>
+  <si>
+    <t>22/04/2020</t>
+  </si>
+  <si>
+    <t>% moyen 1 week (65.0)</t>
+  </si>
+  <si>
+    <t>23/04/2020</t>
+  </si>
+  <si>
+    <t>% 2 weeks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indicateurs : </t>
+  </si>
+  <si>
+    <t>% moyen reco ref (9.0)</t>
+  </si>
+  <si>
+    <t>Pourcentage moyen entre le cours actuel et le cours de ref pour les actions ayant une recommandation</t>
+  </si>
+  <si>
+    <t>% moyen 2 weeks (34.0)</t>
+  </si>
+  <si>
+    <t>Pourcentage moyen entre le cours actuel et le cours d'il y a 2 semaines (Ex : -10% si le cours est passé de 10 (il y a 2 semaines) à 9 (actuel))</t>
+  </si>
+  <si>
+    <t>Top 10</t>
+  </si>
+  <si>
+    <t>% Top 10 baissier 1 week (10)</t>
+  </si>
+  <si>
+    <t>Top 10 des actions ayant le plus baissé depuis 1 semaine</t>
+  </si>
+  <si>
+    <t>% Top 10 haussier 1 week (10)</t>
+  </si>
+  <si>
+    <t>Top 10 des actions ayant le plus monté depuis 1 semaine</t>
+  </si>
+  <si>
+    <t>Short Top</t>
+  </si>
+  <si>
+    <t>% Top 5 baissier ref (5)</t>
+  </si>
+  <si>
+    <t>Top 5 des actions ayant le plus baissé depuis le cours de référence</t>
+  </si>
+  <si>
+    <t>% Top 2 baissier ref (2)</t>
+  </si>
+  <si>
+    <t>Top 2 des actions ayant le plus baissé depuis le cours de référence</t>
+  </si>
+  <si>
+    <t>24/04/2020</t>
+  </si>
+  <si>
+    <t>% moyen baissier ref (57)</t>
+  </si>
+  <si>
+    <t>% moyen 2 weeks (35.0)</t>
   </si>
 </sst>
 </file>
@@ -830,7 +914,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="733">
+  <cellXfs count="520">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -839,491 +923,278 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -1623,7 +1494,7 @@
             <c:strRef>
               <c:f>data!$A$6:$A$20</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>01/12/2019</c:v>
                 </c:pt>
@@ -1647,6 +1518,18 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>17/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>23/04/2020</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1680,6 +1563,18 @@
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
                   <c:v>15.022</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>14.878</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>14.667999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>14.734</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>14.792</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1707,7 +1602,7 @@
             <c:strRef>
               <c:f>data!$A$6:$A$20</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>01/12/2019</c:v>
                 </c:pt>
@@ -1731,6 +1626,18 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>17/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>23/04/2020</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1764,6 +1671,18 @@
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
                   <c:v>14.03</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>13.632</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>13.43</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>13.512</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>13.872</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1791,7 +1710,7 @@
             <c:strRef>
               <c:f>data!$A$6:$A$20</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>01/12/2019</c:v>
                 </c:pt>
@@ -1815,6 +1734,18 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>17/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>23/04/2020</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1848,6 +1779,18 @@
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
                   <c:v>26.035</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>25.01</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>24.85</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>25.535</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>26.835000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1875,7 +1818,7 @@
             <c:strRef>
               <c:f>data!$A$6:$A$20</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>01/12/2019</c:v>
                 </c:pt>
@@ -1899,6 +1842,18 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>17/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>23/04/2020</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1932,6 +1887,18 @@
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
                   <c:v>6.5119999999999996</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>6.4539999999999997</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>6.3639999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>6.476</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>6.6459999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1959,7 +1926,7 @@
             <c:strRef>
               <c:f>data!$A$6:$A$20</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>01/12/2019</c:v>
                 </c:pt>
@@ -1983,6 +1950,18 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>17/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>23/04/2020</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2016,6 +1995,18 @@
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
                   <c:v>26.14</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>25.76</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>26.26</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>25.75</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>26.02</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2043,7 +2034,7 @@
             <c:strRef>
               <c:f>data!$A$6:$A$20</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>01/12/2019</c:v>
                 </c:pt>
@@ -2067,6 +2058,18 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>17/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>23/04/2020</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2100,6 +2103,18 @@
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
                   <c:v>9.5579999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>9.3559999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>9.2100000000000009</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>9.1359999999999992</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>9.1440000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2127,7 +2142,7 @@
             <c:strRef>
               <c:f>data!$A$6:$A$20</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>01/12/2019</c:v>
                 </c:pt>
@@ -2151,6 +2166,18 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>17/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>23/04/2020</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2184,6 +2211,18 @@
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
                   <c:v>24.9</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>24.05</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>23.94</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>24.15</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>23.88</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2211,7 +2250,7 @@
             <c:strRef>
               <c:f>data!$A$6:$A$20</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>01/12/2019</c:v>
                 </c:pt>
@@ -2235,6 +2274,18 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>17/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22/04/2020</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>23/04/2020</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2268,6 +2319,18 @@
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
                   <c:v>13.95</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>13.2</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>14.4</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>14.45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2284,11 +2347,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="193041408"/>
-        <c:axId val="161371200"/>
+        <c:axId val="190685696"/>
+        <c:axId val="160126016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="193041408"/>
+        <c:axId val="190685696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2297,7 +2360,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161371200"/>
+        <c:crossAx val="160126016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2305,7 +2368,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="161371200"/>
+        <c:axId val="160126016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2316,7 +2379,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193041408"/>
+        <c:crossAx val="190685696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2640,7 +2703,7 @@
   <dimension ref="A1:BN20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2657,7 +2720,193 @@
       <c r="B1" t="s">
         <v>137</v>
       </c>
+      <c r="C1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H1" t="s">
+        <v>137</v>
+      </c>
+      <c r="I1" t="s">
+        <v>137</v>
+      </c>
+      <c r="J1" t="s">
+        <v>137</v>
+      </c>
+      <c r="K1" t="s">
+        <v>137</v>
+      </c>
+      <c r="L1" t="s">
+        <v>137</v>
+      </c>
+      <c r="M1" t="s">
+        <v>137</v>
+      </c>
+      <c r="N1" t="s">
+        <v>137</v>
+      </c>
+      <c r="O1" t="s">
+        <v>137</v>
+      </c>
+      <c r="P1" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>137</v>
+      </c>
+      <c r="R1" t="s">
+        <v>137</v>
+      </c>
+      <c r="S1" t="s">
+        <v>137</v>
+      </c>
+      <c r="T1" t="s">
+        <v>137</v>
+      </c>
+      <c r="U1" t="s">
+        <v>137</v>
+      </c>
+      <c r="V1" t="s">
+        <v>137</v>
+      </c>
+      <c r="W1" t="s">
+        <v>137</v>
+      </c>
+      <c r="X1" t="s">
+        <v>137</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>137</v>
+      </c>
       <c r="AO1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>9</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>9</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>9</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>9</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>9</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>9</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>9</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>9</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>9</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>9</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>9</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>9</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>9</v>
+      </c>
+      <c r="BM1" t="s">
         <v>9</v>
       </c>
       <c r="BN1" t="s">
@@ -4596,417 +4845,1008 @@
     </row>
     <row r="14" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="B14" t="n">
+        <v>251</v>
+      </c>
+      <c r="B14">
         <v>14.878</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C14">
         <v>13.632</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D14">
         <v>25.01</v>
       </c>
-      <c r="E14" t="n">
-        <v>6.454</v>
-      </c>
-      <c r="F14" t="n">
+      <c r="E14">
+        <v>6.4539999999999997</v>
+      </c>
+      <c r="F14">
         <v>25.76</v>
       </c>
-      <c r="G14" t="n">
-        <v>9.356</v>
-      </c>
-      <c r="H14" t="n">
+      <c r="G14">
+        <v>9.3559999999999999</v>
+      </c>
+      <c r="H14">
         <v>24.05</v>
       </c>
-      <c r="I14" t="n">
+      <c r="I14">
         <v>13.2</v>
       </c>
-      <c r="J14" t="n">
+      <c r="J14">
         <v>353.7</v>
       </c>
-      <c r="K14" t="n">
+      <c r="K14">
         <v>59.3</v>
       </c>
-      <c r="L14" t="n">
+      <c r="L14">
         <v>21.34</v>
       </c>
-      <c r="M14" t="n">
-        <v>73.18</v>
-      </c>
-      <c r="N14" t="n">
-        <v>19.135</v>
-      </c>
-      <c r="O14" t="n">
-        <v>29.825</v>
-      </c>
-      <c r="P14" t="n">
+      <c r="M14">
+        <v>73.180000000000007</v>
+      </c>
+      <c r="N14">
+        <v>19.135000000000002</v>
+      </c>
+      <c r="O14">
+        <v>29.824999999999999</v>
+      </c>
+      <c r="P14">
         <v>72.16</v>
       </c>
-      <c r="Q14" t="n">
+      <c r="Q14">
         <v>20.66</v>
       </c>
-      <c r="R14" t="n">
-        <v>66.6</v>
-      </c>
-      <c r="S14" t="n">
-        <v>81.82</v>
-      </c>
-      <c r="T14" t="n">
+      <c r="R14">
+        <v>66.599999999999994</v>
+      </c>
+      <c r="S14">
+        <v>81.819999999999993</v>
+      </c>
+      <c r="T14">
         <v>85.52</v>
       </c>
-      <c r="U14" t="n">
-        <v>79.74</v>
-      </c>
-      <c r="V14" t="n">
-        <v>16.336</v>
-      </c>
-      <c r="W14" t="n">
+      <c r="U14">
+        <v>79.739999999999995</v>
+      </c>
+      <c r="V14">
+        <v>16.335999999999999</v>
+      </c>
+      <c r="W14">
         <v>25.5</v>
       </c>
-      <c r="X14" t="n">
+      <c r="X14">
         <v>87.3</v>
       </c>
-      <c r="Y14" t="n">
+      <c r="Y14">
         <v>11.275</v>
       </c>
-      <c r="Z14" t="n">
+      <c r="Z14">
         <v>139.4</v>
       </c>
-      <c r="AA14" t="n">
+      <c r="AA14">
         <v>11.63</v>
       </c>
-      <c r="AB14" t="n">
+      <c r="AB14">
         <v>14.01</v>
       </c>
-      <c r="AC14" t="n">
+      <c r="AC14">
         <v>63.04</v>
       </c>
-      <c r="AD14" t="n">
-        <v>136.7</v>
-      </c>
-      <c r="AE14" t="n">
+      <c r="AD14">
+        <v>136.69999999999999</v>
+      </c>
+      <c r="AE14">
         <v>110.8</v>
       </c>
-      <c r="AF14" t="n">
+      <c r="AF14">
         <v>689.4</v>
       </c>
-      <c r="AG14" t="n">
+      <c r="AG14">
         <v>501.4</v>
       </c>
-      <c r="AH14" t="n">
+      <c r="AH14">
         <v>245.8</v>
       </c>
-      <c r="AI14" t="n">
+      <c r="AI14">
         <v>59.2</v>
       </c>
-      <c r="AJ14" t="n">
+      <c r="AJ14">
         <v>80.92</v>
       </c>
-      <c r="AK14" t="n">
+      <c r="AK14">
         <v>26.41</v>
       </c>
-      <c r="AL14" t="n">
+      <c r="AL14">
         <v>63.6</v>
       </c>
-      <c r="AM14" t="n">
+      <c r="AM14">
         <v>55.26</v>
       </c>
-      <c r="AN14" t="n">
+      <c r="AN14">
         <v>119.55</v>
       </c>
-      <c r="AO14" t="n">
+      <c r="AO14">
         <v>146.38</v>
       </c>
-      <c r="AP14" t="n">
+      <c r="AP14">
         <v>87.38</v>
       </c>
-      <c r="AQ14" t="n">
+      <c r="AQ14">
         <v>282.8</v>
       </c>
-      <c r="AR14" t="n">
-        <v>106.0</v>
-      </c>
-      <c r="AS14" t="n">
+      <c r="AR14">
+        <v>106</v>
+      </c>
+      <c r="AS14">
         <v>87.2</v>
       </c>
-      <c r="AT14" t="n">
+      <c r="AT14">
         <v>42.48</v>
       </c>
-      <c r="AU14" t="n">
+      <c r="AU14">
         <v>48.07</v>
       </c>
-      <c r="AV14" t="n">
-        <v>33.41</v>
-      </c>
-      <c r="AW14" t="n">
+      <c r="AV14">
+        <v>33.409999999999997</v>
+      </c>
+      <c r="AW14">
         <v>43.21</v>
       </c>
-      <c r="AX14" t="n">
+      <c r="AX14">
         <v>183.41</v>
       </c>
-      <c r="AY14" t="n">
+      <c r="AY14">
         <v>209.4</v>
       </c>
-      <c r="AZ14" t="n">
+      <c r="AZ14">
         <v>120.11</v>
       </c>
-      <c r="BA14" t="n">
+      <c r="BA14">
         <v>60.36</v>
       </c>
-      <c r="BB14" t="n">
-        <v>95.0</v>
-      </c>
-      <c r="BC14" t="n">
-        <v>151.92</v>
-      </c>
-      <c r="BD14" t="n">
+      <c r="BB14">
+        <v>95</v>
+      </c>
+      <c r="BC14">
+        <v>151.91999999999999</v>
+      </c>
+      <c r="BD14">
         <v>186.1</v>
       </c>
-      <c r="BE14" t="n">
+      <c r="BE14">
         <v>89.87</v>
       </c>
-      <c r="BF14" t="n">
+      <c r="BF14">
         <v>36.9</v>
       </c>
-      <c r="BG14" t="n">
+      <c r="BG14">
         <v>124.66</v>
       </c>
-      <c r="BH14" t="n">
+      <c r="BH14">
         <v>105.1</v>
       </c>
-      <c r="BI14" t="n">
+      <c r="BI14">
         <v>86.14</v>
       </c>
-      <c r="BJ14" t="n">
+      <c r="BJ14">
         <v>58.47</v>
       </c>
-      <c r="BK14" t="n">
+      <c r="BK14">
         <v>169.37</v>
       </c>
-      <c r="BL14" t="n">
+      <c r="BL14">
         <v>44.5</v>
       </c>
-      <c r="BM14" t="n">
+      <c r="BM14">
         <v>106.65</v>
       </c>
-      <c r="BN14" t="n">
+      <c r="BN14">
         <v>56.6</v>
       </c>
     </row>
     <row r="15" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="B15" t="n">
-        <v>14.668</v>
-      </c>
-      <c r="C15" t="n">
+        <v>252</v>
+      </c>
+      <c r="B15">
+        <v>14.667999999999999</v>
+      </c>
+      <c r="C15">
         <v>13.43</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D15">
         <v>24.85</v>
       </c>
-      <c r="E15" t="n">
-        <v>6.364</v>
-      </c>
-      <c r="F15" t="n">
+      <c r="E15">
+        <v>6.3639999999999999</v>
+      </c>
+      <c r="F15">
         <v>26.26</v>
       </c>
-      <c r="G15" t="n">
-        <v>9.21</v>
-      </c>
-      <c r="H15" t="n">
+      <c r="G15">
+        <v>9.2100000000000009</v>
+      </c>
+      <c r="H15">
         <v>23.94</v>
       </c>
-      <c r="I15" t="n">
-        <v>13.0</v>
-      </c>
-      <c r="J15" t="n">
+      <c r="I15">
+        <v>13</v>
+      </c>
+      <c r="J15">
         <v>354.45</v>
       </c>
-      <c r="K15" t="n">
+      <c r="K15">
         <v>59.64</v>
       </c>
-      <c r="L15" t="n">
+      <c r="L15">
         <v>20.69</v>
       </c>
-      <c r="M15" t="n">
+      <c r="M15">
         <v>72.28</v>
       </c>
-      <c r="N15" t="n">
+      <c r="N15">
         <v>17.785</v>
       </c>
-      <c r="O15" t="n">
+      <c r="O15">
         <v>29.48</v>
       </c>
-      <c r="P15" t="n">
-        <v>71.46</v>
-      </c>
-      <c r="Q15" t="n">
+      <c r="P15">
+        <v>71.459999999999994</v>
+      </c>
+      <c r="Q15">
         <v>20.58</v>
       </c>
-      <c r="R15" t="n">
-        <v>66.9</v>
-      </c>
-      <c r="S15" t="n">
+      <c r="R15">
+        <v>66.900000000000006</v>
+      </c>
+      <c r="S15">
         <v>82.38</v>
       </c>
-      <c r="T15" t="n">
+      <c r="T15">
         <v>88.39</v>
       </c>
-      <c r="U15" t="n">
+      <c r="U15">
         <v>76.88</v>
       </c>
-      <c r="V15" t="n">
-        <v>16.222</v>
-      </c>
-      <c r="W15" t="n">
+      <c r="V15">
+        <v>16.222000000000001</v>
+      </c>
+      <c r="W15">
         <v>25.23</v>
       </c>
-      <c r="X15" t="n">
+      <c r="X15">
         <v>86.82</v>
       </c>
-      <c r="Y15" t="n">
+      <c r="Y15">
         <v>11.18</v>
       </c>
-      <c r="Z15" t="n">
-        <v>139.0</v>
-      </c>
-      <c r="AA15" t="n">
+      <c r="Z15">
+        <v>139</v>
+      </c>
+      <c r="AA15">
         <v>11.68</v>
       </c>
-      <c r="AB15" t="n">
+      <c r="AB15">
         <v>13.855</v>
       </c>
-      <c r="AC15" t="n">
+      <c r="AC15">
         <v>63.24</v>
       </c>
-      <c r="AD15" t="n">
+      <c r="AD15">
         <v>135.1</v>
       </c>
-      <c r="AE15" t="n">
-        <v>108.0</v>
-      </c>
-      <c r="AF15" t="n">
+      <c r="AE15">
+        <v>108</v>
+      </c>
+      <c r="AF15">
         <v>684.6</v>
       </c>
-      <c r="AG15" t="n">
+      <c r="AG15">
         <v>497.8</v>
       </c>
-      <c r="AH15" t="n">
+      <c r="AH15">
         <v>254.8</v>
       </c>
-      <c r="AI15" t="n">
+      <c r="AI15">
         <v>55.96</v>
       </c>
-      <c r="AJ15" t="n">
-        <v>80.54</v>
-      </c>
-      <c r="AK15" t="n">
+      <c r="AJ15">
+        <v>80.540000000000006</v>
+      </c>
+      <c r="AK15">
         <v>25.59</v>
       </c>
-      <c r="AL15" t="n">
+      <c r="AL15">
         <v>64.78</v>
       </c>
-      <c r="AM15" t="n">
+      <c r="AM15">
         <v>53.02</v>
       </c>
-      <c r="AN15" t="n">
+      <c r="AN15">
         <v>119.4</v>
       </c>
-      <c r="AO15" t="n">
-        <v>143.7</v>
-      </c>
-      <c r="AP15" t="n">
+      <c r="AO15">
+        <v>143.69999999999999</v>
+      </c>
+      <c r="AP15">
         <v>84.01</v>
       </c>
-      <c r="AQ15" t="n">
+      <c r="AQ15">
         <v>276.93</v>
       </c>
-      <c r="AR15" t="n">
+      <c r="AR15">
         <v>106.5</v>
       </c>
-      <c r="AS15" t="n">
+      <c r="AS15">
         <v>83.51</v>
       </c>
-      <c r="AT15" t="n">
+      <c r="AT15">
         <v>42.54</v>
       </c>
-      <c r="AU15" t="n">
+      <c r="AU15">
         <v>46.59</v>
       </c>
-      <c r="AV15" t="n">
+      <c r="AV15">
         <v>31.53</v>
       </c>
-      <c r="AW15" t="n">
+      <c r="AW15">
         <v>41.18</v>
       </c>
-      <c r="AX15" t="n">
+      <c r="AX15">
         <v>180.5</v>
       </c>
-      <c r="AY15" t="n">
+      <c r="AY15">
         <v>206.16</v>
       </c>
-      <c r="AZ15" t="n">
+      <c r="AZ15">
         <v>120.58</v>
       </c>
-      <c r="BA15" t="n">
+      <c r="BA15">
         <v>59.18</v>
       </c>
-      <c r="BB15" t="n">
+      <c r="BB15">
         <v>91.64</v>
       </c>
-      <c r="BC15" t="n">
-        <v>151.83</v>
-      </c>
-      <c r="BD15" t="n">
+      <c r="BC15">
+        <v>151.83000000000001</v>
+      </c>
+      <c r="BD15">
         <v>181.7</v>
       </c>
-      <c r="BE15" t="n">
+      <c r="BE15">
         <v>87.86</v>
       </c>
-      <c r="BF15" t="n">
+      <c r="BF15">
         <v>36.08</v>
       </c>
-      <c r="BG15" t="n">
+      <c r="BG15">
         <v>120.58</v>
       </c>
-      <c r="BH15" t="n">
+      <c r="BH15">
         <v>101.75</v>
       </c>
-      <c r="BI15" t="n">
+      <c r="BI15">
         <v>86.14</v>
       </c>
-      <c r="BJ15" t="n">
+      <c r="BJ15">
         <v>58.15</v>
       </c>
-      <c r="BK15" t="n">
+      <c r="BK15">
         <v>164.22</v>
       </c>
-      <c r="BL15" t="n">
+      <c r="BL15">
         <v>42.85</v>
       </c>
-      <c r="BM15" t="n">
+      <c r="BM15">
         <v>102.21</v>
       </c>
-      <c r="BN15" t="n">
+      <c r="BN15">
         <v>56.97</v>
       </c>
     </row>
     <row r="16" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="B16">
+        <v>14.734</v>
+      </c>
+      <c r="C16">
+        <v>13.512</v>
+      </c>
+      <c r="D16">
+        <v>25.535</v>
+      </c>
+      <c r="E16">
+        <v>6.476</v>
+      </c>
+      <c r="F16">
+        <v>25.75</v>
+      </c>
+      <c r="G16">
+        <v>9.1359999999999992</v>
+      </c>
+      <c r="H16">
+        <v>24.15</v>
+      </c>
+      <c r="I16">
+        <v>14.4</v>
+      </c>
+      <c r="J16">
+        <v>353.45</v>
+      </c>
+      <c r="K16">
+        <v>59.98</v>
+      </c>
+      <c r="L16">
+        <v>20.32</v>
+      </c>
+      <c r="M16">
+        <v>71.88</v>
+      </c>
+      <c r="N16">
+        <v>17.98</v>
+      </c>
+      <c r="O16">
+        <v>31.114999999999998</v>
+      </c>
+      <c r="P16">
+        <v>70</v>
+      </c>
+      <c r="Q16">
+        <v>21.4</v>
+      </c>
+      <c r="R16">
+        <v>65.14</v>
+      </c>
+      <c r="S16">
+        <v>82.56</v>
+      </c>
+      <c r="T16">
+        <v>88.16</v>
+      </c>
+      <c r="U16">
+        <v>75</v>
+      </c>
+      <c r="V16">
+        <v>15.83</v>
+      </c>
+      <c r="W16">
+        <v>24.65</v>
+      </c>
+      <c r="X16">
+        <v>83.78</v>
+      </c>
+      <c r="Y16">
+        <v>11.305</v>
+      </c>
+      <c r="Z16">
+        <v>136.5</v>
+      </c>
+      <c r="AA16">
+        <v>12.38</v>
+      </c>
+      <c r="AB16">
+        <v>13.79</v>
+      </c>
+      <c r="AC16">
+        <v>62.4</v>
+      </c>
+      <c r="AD16">
+        <v>137.75</v>
+      </c>
+      <c r="AE16">
+        <v>104.7</v>
+      </c>
+      <c r="AF16">
+        <v>672.6</v>
+      </c>
+      <c r="AG16">
+        <v>464.95</v>
+      </c>
+      <c r="AH16">
+        <v>248.1</v>
+      </c>
+      <c r="AI16">
+        <v>58.2</v>
+      </c>
+      <c r="AJ16">
+        <v>80.3</v>
+      </c>
+      <c r="AK16">
+        <v>26.17</v>
+      </c>
+      <c r="AL16">
+        <v>61.84</v>
+      </c>
+      <c r="AM16">
+        <v>53.53</v>
+      </c>
+      <c r="AN16">
+        <v>117.45</v>
+      </c>
+      <c r="AO16">
+        <v>142.6</v>
+      </c>
+      <c r="AP16">
+        <v>82.715000000000003</v>
+      </c>
+      <c r="AQ16">
+        <v>276.48500000000001</v>
+      </c>
+      <c r="AR16">
+        <v>106.5</v>
+      </c>
+      <c r="AS16">
+        <v>84.52</v>
+      </c>
+      <c r="AT16">
+        <v>41.655000000000001</v>
+      </c>
+      <c r="AU16">
+        <v>45.704999999999998</v>
+      </c>
+      <c r="AV16">
+        <v>31.494</v>
+      </c>
+      <c r="AW16">
+        <v>42.145000000000003</v>
+      </c>
+      <c r="AX16">
+        <v>175.56</v>
+      </c>
+      <c r="AY16">
+        <v>205.34</v>
+      </c>
+      <c r="AZ16">
+        <v>119.49</v>
+      </c>
+      <c r="BA16">
+        <v>60.03</v>
+      </c>
+      <c r="BB16">
+        <v>89.84</v>
+      </c>
+      <c r="BC16">
+        <v>153.47999999999999</v>
+      </c>
+      <c r="BD16">
+        <v>186.6</v>
+      </c>
+      <c r="BE16">
+        <v>89.09</v>
+      </c>
+      <c r="BF16">
+        <v>36.35</v>
+      </c>
+      <c r="BG16">
+        <v>119.78</v>
+      </c>
+      <c r="BH16">
+        <v>101.5</v>
+      </c>
+      <c r="BI16">
+        <v>86.14</v>
+      </c>
+      <c r="BJ16">
+        <v>58.085000000000001</v>
+      </c>
+      <c r="BK16">
+        <v>166.25399999999999</v>
+      </c>
+      <c r="BL16">
+        <v>43.19</v>
+      </c>
+      <c r="BM16">
+        <v>101.6</v>
+      </c>
+      <c r="BN16">
+        <v>55.866900000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="B17">
+        <v>14.792</v>
+      </c>
+      <c r="C17">
+        <v>13.872</v>
+      </c>
+      <c r="D17">
+        <v>26.835000000000001</v>
+      </c>
+      <c r="E17">
+        <v>6.6459999999999999</v>
+      </c>
+      <c r="F17">
+        <v>26.02</v>
+      </c>
+      <c r="G17">
+        <v>9.1440000000000001</v>
+      </c>
+      <c r="H17">
+        <v>23.88</v>
+      </c>
+      <c r="I17">
+        <v>14.45</v>
+      </c>
+      <c r="J17">
+        <v>348.15</v>
+      </c>
+      <c r="K17">
+        <v>62.76</v>
+      </c>
+      <c r="L17">
+        <v>20</v>
+      </c>
+      <c r="M17">
+        <v>69.94</v>
+      </c>
+      <c r="N17">
+        <v>18.465</v>
+      </c>
+      <c r="O17">
+        <v>31.975000000000001</v>
+      </c>
+      <c r="P17">
+        <v>68.44</v>
+      </c>
+      <c r="Q17">
+        <v>21.76</v>
+      </c>
+      <c r="R17">
+        <v>64.86</v>
+      </c>
+      <c r="S17">
+        <v>83.04</v>
+      </c>
+      <c r="T17">
+        <v>89.91</v>
+      </c>
+      <c r="U17">
+        <v>75.3</v>
+      </c>
+      <c r="V17">
+        <v>16.006</v>
+      </c>
+      <c r="W17">
+        <v>25.43</v>
+      </c>
+      <c r="X17">
+        <v>82.68</v>
+      </c>
+      <c r="Y17">
+        <v>11.385</v>
+      </c>
+      <c r="Z17">
+        <v>137.35</v>
+      </c>
+      <c r="AA17">
+        <v>12.45</v>
+      </c>
+      <c r="AB17">
+        <v>13.57</v>
+      </c>
+      <c r="AC17">
+        <v>61.92</v>
+      </c>
+      <c r="AD17">
+        <v>136.80000000000001</v>
+      </c>
+      <c r="AE17">
+        <v>106.4</v>
+      </c>
+      <c r="AF17">
+        <v>687.2</v>
+      </c>
+      <c r="AG17">
+        <v>454.6</v>
+      </c>
+      <c r="AH17">
+        <v>246.3</v>
+      </c>
+      <c r="AI17">
+        <v>59.56</v>
+      </c>
+      <c r="AJ17">
+        <v>79.56</v>
+      </c>
+      <c r="AK17">
+        <v>26.48</v>
+      </c>
+      <c r="AL17">
+        <v>61.12</v>
+      </c>
+      <c r="AM17">
+        <v>53.2</v>
+      </c>
+      <c r="AN17">
+        <v>117</v>
+      </c>
+      <c r="AO17">
+        <v>143.62</v>
+      </c>
+      <c r="AP17">
+        <v>82.55</v>
+      </c>
+      <c r="AQ17">
+        <v>276.10000000000002</v>
+      </c>
+      <c r="AR17">
+        <v>106.5</v>
+      </c>
+      <c r="AS17">
+        <v>84.44</v>
+      </c>
+      <c r="AT17">
+        <v>41.76</v>
+      </c>
+      <c r="AU17">
+        <v>45.6</v>
+      </c>
+      <c r="AV17">
+        <v>31.84</v>
+      </c>
+      <c r="AW17">
+        <v>42.11</v>
+      </c>
+      <c r="AX17">
+        <v>175.98</v>
+      </c>
+      <c r="AY17">
+        <v>204.11</v>
+      </c>
+      <c r="AZ17">
+        <v>119.33</v>
+      </c>
+      <c r="BA17">
+        <v>60.1</v>
+      </c>
+      <c r="BB17">
+        <v>89.33</v>
+      </c>
+      <c r="BC17">
+        <v>153</v>
+      </c>
+      <c r="BD17">
+        <v>186.52</v>
+      </c>
+      <c r="BE17">
+        <v>88.775000000000006</v>
+      </c>
+      <c r="BF17">
+        <v>36.24</v>
+      </c>
+      <c r="BG17">
+        <v>119.41</v>
+      </c>
+      <c r="BH17">
+        <v>101.7</v>
+      </c>
+      <c r="BI17">
+        <v>86.14</v>
+      </c>
+      <c r="BJ17">
+        <v>57.96</v>
+      </c>
+      <c r="BK17">
+        <v>166.55</v>
+      </c>
+      <c r="BL17">
+        <v>43.31</v>
+      </c>
+      <c r="BM17">
+        <v>101</v>
+      </c>
+      <c r="BN17">
+        <v>55.92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="B18" t="n">
+        <v>14.626</v>
+      </c>
+      <c r="C18" t="n">
+        <v>13.8</v>
+      </c>
+      <c r="D18" t="n">
+        <v>26.455</v>
+      </c>
+      <c r="E18" t="n">
+        <v>6.656</v>
+      </c>
+      <c r="F18" t="n">
+        <v>25.03</v>
+      </c>
+      <c r="G18" t="n">
+        <v>9.168</v>
+      </c>
+      <c r="H18" t="n">
+        <v>23.38</v>
+      </c>
+      <c r="I18" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="J18" t="n">
+        <v>345.5</v>
+      </c>
+      <c r="K18" t="n">
+        <v>66.82</v>
+      </c>
+      <c r="L18" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="M18" t="n">
+        <v>69.92</v>
+      </c>
+      <c r="N18" t="n">
+        <v>18.895</v>
+      </c>
+      <c r="O18" t="n">
+        <v>32.28</v>
+      </c>
+      <c r="P18" t="n">
+        <v>68.56</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>23.03</v>
+      </c>
+      <c r="R18" t="n">
+        <v>67.12</v>
+      </c>
+      <c r="S18" t="n">
+        <v>82.0</v>
+      </c>
+      <c r="T18" t="n">
+        <v>90.17</v>
+      </c>
+      <c r="U18" t="n">
+        <v>76.3</v>
+      </c>
+      <c r="V18" t="n">
+        <v>16.456</v>
+      </c>
+      <c r="W18" t="n">
+        <v>26.89</v>
+      </c>
+      <c r="X18" t="n">
+        <v>82.34</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>11.32</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>135.65</v>
+      </c>
+      <c r="AA18" t="n">
+        <v>12.575</v>
+      </c>
+      <c r="AB18" t="n">
+        <v>13.385</v>
+      </c>
+      <c r="AC18" t="n">
+        <v>62.6</v>
+      </c>
+      <c r="AD18" t="n">
+        <v>136.15</v>
+      </c>
+      <c r="AE18" t="n">
+        <v>105.05</v>
+      </c>
+      <c r="AF18" t="n">
+        <v>681.4</v>
+      </c>
+      <c r="AG18" t="n">
+        <v>447.9</v>
+      </c>
+      <c r="AH18" t="n">
+        <v>243.6</v>
+      </c>
+      <c r="AI18" t="n">
+        <v>58.92</v>
+      </c>
+      <c r="AJ18" t="n">
+        <v>77.86</v>
+      </c>
+      <c r="AK18" t="n">
+        <v>27.02</v>
+      </c>
+      <c r="AL18" t="n">
+        <v>62.54</v>
+      </c>
+      <c r="AM18" t="n">
+        <v>52.96</v>
+      </c>
+      <c r="AN18" t="n">
+        <v>117.1</v>
+      </c>
+      <c r="AO18" t="n">
+        <v>144.33</v>
+      </c>
+      <c r="AP18" t="n">
+        <v>82.51</v>
+      </c>
+      <c r="AQ18" t="n">
+        <v>275.03</v>
+      </c>
+      <c r="AR18" t="n">
+        <v>106.5</v>
+      </c>
+      <c r="AS18" t="n">
+        <v>86.82</v>
+      </c>
+      <c r="AT18" t="n">
+        <v>41.62</v>
+      </c>
+      <c r="AU18" t="n">
+        <v>45.06</v>
+      </c>
+      <c r="AV18" t="n">
+        <v>32.55</v>
+      </c>
+      <c r="AW18" t="n">
+        <v>43.45</v>
+      </c>
+      <c r="AX18" t="n">
+        <v>175.05</v>
+      </c>
+      <c r="AY18" t="n">
+        <v>202.26</v>
+      </c>
+      <c r="AZ18" t="n">
+        <v>121.4</v>
+      </c>
+      <c r="BA18" t="n">
+        <v>59.04</v>
+      </c>
+      <c r="BB18" t="n">
+        <v>89.31</v>
+      </c>
+      <c r="BC18" t="n">
+        <v>155.75</v>
+      </c>
+      <c r="BD18" t="n">
+        <v>182.04</v>
+      </c>
+      <c r="BE18" t="n">
+        <v>87.35</v>
+      </c>
+      <c r="BF18" t="n">
+        <v>36.7</v>
+      </c>
+      <c r="BG18" t="n">
+        <v>119.4</v>
+      </c>
+      <c r="BH18" t="n">
+        <v>100.41</v>
+      </c>
+      <c r="BI18" t="n">
+        <v>86.14</v>
+      </c>
+      <c r="BJ18" t="n">
+        <v>57.7</v>
+      </c>
+      <c r="BK18" t="n">
+        <v>166.27</v>
+      </c>
+      <c r="BL18" t="n">
+        <v>43.5</v>
+      </c>
+      <c r="BM18" t="n">
+        <v>100.9</v>
+      </c>
+      <c r="BN18" t="n">
+        <v>55.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
     </row>
   </sheetData>
@@ -5054,931 +5894,1129 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C1" t="s">
+        <v>263</v>
+      </c>
+      <c r="D1" t="s">
+        <v>249</v>
+      </c>
+      <c r="E1" t="s">
         <v>250</v>
       </c>
-      <c r="D1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="568" t="n">
+      <c r="B2" s="280" t="n">
         <v>-0.41</v>
       </c>
-      <c r="C2" t="n" s="569">
-        <v>-0.06</v>
-      </c>
-      <c r="D2" t="n" s="570">
-        <v>-0.02</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="281" t="n">
+        <v>-0.04</v>
+      </c>
+      <c r="D2" s="282" t="n">
+        <v>-0.03</v>
+      </c>
+      <c r="E2" s="283" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="571" t="n">
-        <v>-0.53</v>
-      </c>
-      <c r="C3" t="n" s="572">
-        <v>-0.11</v>
-      </c>
-      <c r="D3" t="n" s="573">
-        <v>-0.04</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="284" t="n">
+        <v>-0.52</v>
+      </c>
+      <c r="C3" s="285" t="n">
+        <v>-0.06</v>
+      </c>
+      <c r="D3" s="286" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="E3" s="287" t="n">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="574" t="n">
-        <v>-0.51</v>
-      </c>
-      <c r="C4" t="n" s="575">
-        <v>-0.12</v>
-      </c>
-      <c r="D4" t="n" s="576">
-        <v>-0.05</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="288" t="n">
+        <v>-0.48</v>
+      </c>
+      <c r="C4" s="289" t="n">
+        <v>-0.06</v>
+      </c>
+      <c r="D4" s="290" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E4" s="291" t="n">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="577" t="n">
-        <v>-0.49</v>
-      </c>
-      <c r="C5" t="n" s="578">
-        <v>-0.07</v>
-      </c>
-      <c r="D5" t="n" s="579">
-        <v>-0.02</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="292" t="n">
+        <v>-0.47</v>
+      </c>
+      <c r="C5" s="293" t="n">
+        <v>-0.03</v>
+      </c>
+      <c r="D5" s="294" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E5" s="295" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>78</v>
       </c>
-      <c r="B6" s="580" t="n">
-        <v>-0.32</v>
-      </c>
-      <c r="C6" t="n" s="581">
-        <v>-0.06</v>
-      </c>
-      <c r="D6" t="n" s="582">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="296" t="n">
+        <v>-0.35</v>
+      </c>
+      <c r="C6" s="297" t="n">
+        <v>-0.12</v>
+      </c>
+      <c r="D6" s="298" t="n">
+        <v>-0.04</v>
+      </c>
+      <c r="E6" s="299" t="n">
+        <v>-0.03</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="583" t="n">
-        <v>-0.36</v>
-      </c>
-      <c r="C7" t="n" s="584">
-        <v>-0.06</v>
-      </c>
-      <c r="D7" t="n" s="585">
+      <c r="B7" s="300" t="n">
+        <v>-0.37</v>
+      </c>
+      <c r="C7" s="301" t="n">
+        <v>-0.05</v>
+      </c>
+      <c r="D7" s="302" t="n">
         <v>-0.04</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E7" s="303" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="586" t="n">
-        <v>-0.35</v>
-      </c>
-      <c r="C8" t="n" s="587">
+      <c r="B8" s="304" t="n">
+        <v>-0.36</v>
+      </c>
+      <c r="C8" s="305" t="n">
+        <v>-0.09</v>
+      </c>
+      <c r="D8" s="306" t="n">
         <v>-0.06</v>
       </c>
-      <c r="D8" t="n" s="588">
-        <v>-0.04</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E8" s="307" t="n">
+        <v>-0.03</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>84</v>
       </c>
-      <c r="B9" s="589" t="n">
-        <v>-0.61</v>
-      </c>
-      <c r="C9" t="n" s="590">
-        <v>-0.13</v>
-      </c>
-      <c r="D9" t="n" s="591">
-        <v>-0.07</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="308" t="n">
+        <v>-0.53</v>
+      </c>
+      <c r="C9" s="309" t="n">
+        <v>-0.05</v>
+      </c>
+      <c r="D9" s="310" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="E9" s="311" t="n">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>150</v>
       </c>
-      <c r="B10" s="592" t="n">
-        <v>-0.13</v>
-      </c>
-      <c r="C10" t="n" s="593">
-        <v>0.0</v>
-      </c>
-      <c r="D10" t="n" s="594">
+      <c r="B10" s="312" t="n">
+        <v>-0.15</v>
+      </c>
+      <c r="C10" s="313" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D10" s="314" t="n">
+        <v>-0.04</v>
+      </c>
+      <c r="E10" s="315" t="n">
         <v>-0.02</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>185</v>
       </c>
-      <c r="B11" s="595" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="C11" t="s">
-        <v>249</v>
-      </c>
-      <c r="D11" t="n" s="596">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="316" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="D11" s="317" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="E11" s="318" t="n">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>187</v>
       </c>
-      <c r="B12" s="597" t="n">
-        <v>-0.17</v>
-      </c>
-      <c r="C12" t="s">
-        <v>249</v>
-      </c>
-      <c r="D12" t="n" s="598">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="319" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="D12" s="320" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="E12" s="321" t="n">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>189</v>
       </c>
-      <c r="B13" s="599" t="n">
-        <v>-0.27</v>
-      </c>
-      <c r="C13" t="s">
-        <v>249</v>
-      </c>
-      <c r="D13" t="n" s="600">
-        <v>-0.06</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="322" t="n">
+        <v>-0.29</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="D13" s="323" t="n">
+        <v>-0.09</v>
+      </c>
+      <c r="E13" s="324" t="n">
+        <v>-0.03</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>191</v>
       </c>
-      <c r="B14" s="601" t="n">
-        <v>-0.24</v>
-      </c>
-      <c r="C14" t="s">
-        <v>249</v>
-      </c>
-      <c r="D14" t="n" s="602">
-        <v>-0.12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="325" t="n">
+        <v>-0.19</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="D14" s="326" t="n">
+        <v>-0.07</v>
+      </c>
+      <c r="E14" s="327" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>193</v>
       </c>
-      <c r="B15" s="603" t="n">
-        <v>-0.38</v>
-      </c>
-      <c r="C15" t="s">
-        <v>249</v>
-      </c>
-      <c r="D15" t="n" s="604">
-        <v>-0.06</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="328" t="n">
+        <v>-0.32</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="D15" s="329" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="E15" s="330" t="n">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>195</v>
       </c>
-      <c r="B16" s="605" t="n">
-        <v>-0.2</v>
-      </c>
-      <c r="C16" t="s">
-        <v>249</v>
-      </c>
-      <c r="D16" t="n" s="606">
+      <c r="B16" s="331" t="n">
+        <v>-0.23</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="D16" s="332" t="n">
+        <v>-0.06</v>
+      </c>
+      <c r="E16" s="333" t="n">
         <v>-0.02</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>197</v>
       </c>
-      <c r="B17" s="607" t="n">
-        <v>-0.08</v>
-      </c>
-      <c r="C17" t="s">
-        <v>249</v>
-      </c>
-      <c r="D17" t="n" s="608">
-        <v>-0.04</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="334" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="D17" s="335" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="E17" s="336" t="n">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>199</v>
       </c>
-      <c r="B18" s="609" t="n">
+      <c r="B18" s="337" t="n">
         <v>-0.37</v>
       </c>
-      <c r="C18" t="s">
-        <v>249</v>
-      </c>
-      <c r="D18" t="n" s="610">
+      <c r="C18" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="D18" s="338" t="n">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E18" s="339" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>201</v>
       </c>
-      <c r="B19" s="611" t="n">
+      <c r="B19" s="340" t="n">
         <v>-0.06</v>
       </c>
-      <c r="C19" t="s">
-        <v>249</v>
-      </c>
-      <c r="D19" t="n" s="612">
+      <c r="C19" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="D19" s="341" t="n">
         <v>-0.02</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E19" s="342" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>203</v>
       </c>
-      <c r="B20" s="613" t="n">
+      <c r="B20" s="343" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="D20" s="344" t="n">
         <v>0.04</v>
       </c>
-      <c r="C20" t="s">
-        <v>249</v>
-      </c>
-      <c r="D20" t="n" s="614">
+      <c r="E20" s="345" t="n">
         <v>0.02</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>205</v>
       </c>
-      <c r="B21" s="615" t="n">
-        <v>-0.48</v>
-      </c>
-      <c r="C21" t="s">
-        <v>249</v>
-      </c>
-      <c r="D21" t="n" s="616">
-        <v>-0.06</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="346" t="n">
+        <v>-0.49</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>248</v>
+      </c>
+      <c r="D21" s="347" t="n">
+        <v>-0.07</v>
+      </c>
+      <c r="E21" s="348" t="n">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>207</v>
       </c>
-      <c r="B22" s="617" t="n">
-        <v>-0.63</v>
-      </c>
-      <c r="C22" t="s">
-        <v>249</v>
-      </c>
-      <c r="D22" t="n" s="618">
-        <v>-0.02</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="349" t="n">
+        <v>-0.62</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="D22" s="350" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="E22" s="351" t="n">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>209</v>
       </c>
-      <c r="B23" s="619" t="n">
-        <v>-0.37</v>
-      </c>
-      <c r="C23" t="s">
-        <v>249</v>
-      </c>
-      <c r="D23" t="n" s="620">
-        <v>-0.04</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="352" t="n">
+        <v>-0.33</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="D23" s="353" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E23" s="354" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>211</v>
       </c>
-      <c r="B24" s="621" t="n">
-        <v>-0.2</v>
-      </c>
-      <c r="C24" t="s">
-        <v>249</v>
-      </c>
-      <c r="D24" t="n" s="622">
-        <v>-0.03</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="355" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>248</v>
+      </c>
+      <c r="D24" s="356" t="n">
+        <v>-0.08</v>
+      </c>
+      <c r="E24" s="357" t="n">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>213</v>
       </c>
-      <c r="B25" s="623" t="n">
+      <c r="B25" s="358" t="n">
         <v>-0.24</v>
       </c>
-      <c r="C25" t="s">
-        <v>249</v>
-      </c>
-      <c r="D25" t="n" s="624">
-        <v>-0.02</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="D25" s="359" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="E25" s="360" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>215</v>
       </c>
-      <c r="B26" s="625" t="n">
-        <v>-0.16</v>
-      </c>
-      <c r="C26" t="s">
-        <v>249</v>
-      </c>
-      <c r="D26" t="n" s="626">
+      <c r="B26" s="361" t="n">
+        <v>-0.18</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>248</v>
+      </c>
+      <c r="D26" s="362" t="n">
+        <v>-0.03</v>
+      </c>
+      <c r="E26" s="363" t="n">
         <v>-0.01</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>217</v>
       </c>
-      <c r="B27" s="627" t="n">
-        <v>-0.47</v>
-      </c>
-      <c r="C27" t="s">
-        <v>249</v>
-      </c>
-      <c r="D27" t="n" s="628">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="364" t="n">
+        <v>-0.43</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>248</v>
+      </c>
+      <c r="D27" s="365" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="E27" s="366" t="n">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>219</v>
       </c>
-      <c r="B28" s="629" t="n">
-        <v>-0.08</v>
-      </c>
-      <c r="C28" t="s">
-        <v>249</v>
-      </c>
-      <c r="D28" t="n" s="630">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="367" t="n">
+        <v>-0.11</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>248</v>
+      </c>
+      <c r="D28" s="368" t="n">
+        <v>-0.04</v>
+      </c>
+      <c r="E28" s="369" t="n">
+        <v>-0.03</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>221</v>
       </c>
-      <c r="B29" s="631" t="n">
-        <v>-0.15</v>
-      </c>
-      <c r="C29" t="s">
-        <v>249</v>
-      </c>
-      <c r="D29" t="n" s="632">
-        <v>-0.01</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="370" t="n">
+        <v>-0.16</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="D29" s="371" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="E29" s="372" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>223</v>
       </c>
-      <c r="B30" s="633" t="n">
-        <v>-0.06</v>
-      </c>
-      <c r="C30" t="s">
-        <v>249</v>
-      </c>
-      <c r="D30" t="n" s="634">
-        <v>-0.04</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="373" t="n">
+        <v>-0.05</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>248</v>
+      </c>
+      <c r="D30" s="374" t="n">
+        <v>-0.03</v>
+      </c>
+      <c r="E30" s="375" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>225</v>
       </c>
-      <c r="B31" s="635" t="n">
-        <v>-0.23</v>
-      </c>
-      <c r="C31" t="s">
-        <v>249</v>
-      </c>
-      <c r="D31" t="n" s="636">
+      <c r="B31" s="376" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="C31" s="30" t="s">
+        <v>248</v>
+      </c>
+      <c r="D31" s="377" t="n">
+        <v>-0.03</v>
+      </c>
+      <c r="E31" s="378" t="n">
         <v>0.0</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>227</v>
       </c>
-      <c r="B32" s="637" t="n">
+      <c r="B32" s="379" t="n">
         <v>0.0</v>
       </c>
-      <c r="C32" t="s">
-        <v>249</v>
-      </c>
-      <c r="D32" t="n" s="638">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" s="31" t="s">
+        <v>248</v>
+      </c>
+      <c r="D32" s="380" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="E32" s="381" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>229</v>
       </c>
-      <c r="B33" s="639" t="n">
-        <v>-0.09</v>
-      </c>
-      <c r="C33" t="s">
-        <v>249</v>
-      </c>
-      <c r="D33" t="n" s="640">
-        <v>-0.02</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="382" t="n">
+        <v>-0.18</v>
+      </c>
+      <c r="C33" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="D33" s="383" t="n">
+        <v>-0.12</v>
+      </c>
+      <c r="E33" s="384" t="n">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>231</v>
       </c>
-      <c r="B34" s="641" t="n">
-        <v>-0.01</v>
-      </c>
-      <c r="C34" t="s">
-        <v>249</v>
-      </c>
-      <c r="D34" t="n" s="642">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="385" t="n">
+        <v>-0.06</v>
+      </c>
+      <c r="C34" s="33" t="s">
+        <v>248</v>
+      </c>
+      <c r="D34" s="386" t="n">
+        <v>-0.03</v>
+      </c>
+      <c r="E34" s="387" t="n">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>233</v>
       </c>
-      <c r="B35" s="643" t="n">
-        <v>-0.22</v>
-      </c>
-      <c r="C35" t="s">
-        <v>249</v>
-      </c>
-      <c r="D35" t="n" s="644">
-        <v>-0.07</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="388" t="n">
+        <v>-0.18</v>
+      </c>
+      <c r="C35" s="34" t="s">
+        <v>248</v>
+      </c>
+      <c r="D35" s="389" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="E35" s="390" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>235</v>
       </c>
-      <c r="B36" s="645" t="n">
-        <v>-0.25</v>
-      </c>
-      <c r="C36" t="s">
-        <v>249</v>
-      </c>
-      <c r="D36" t="n" s="646">
-        <v>-0.02</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="391" t="n">
+        <v>-0.27</v>
+      </c>
+      <c r="C36" s="35" t="s">
+        <v>248</v>
+      </c>
+      <c r="D36" s="392" t="n">
+        <v>-0.05</v>
+      </c>
+      <c r="E36" s="393" t="n">
+        <v>-0.03</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>237</v>
       </c>
-      <c r="B37" s="647" t="n">
-        <v>-0.31</v>
-      </c>
-      <c r="C37" t="s">
-        <v>249</v>
-      </c>
-      <c r="D37" t="n" s="648">
-        <v>-0.05</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="394" t="n">
+        <v>-0.27</v>
+      </c>
+      <c r="C37" s="36" t="s">
+        <v>248</v>
+      </c>
+      <c r="D37" s="395" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E37" s="396" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>239</v>
       </c>
-      <c r="B38" s="649" t="n">
-        <v>-0.16</v>
-      </c>
-      <c r="C38" t="s">
-        <v>249</v>
-      </c>
-      <c r="D38" t="n" s="650">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="397" t="n">
+        <v>-0.19</v>
+      </c>
+      <c r="C38" s="37" t="s">
+        <v>248</v>
+      </c>
+      <c r="D38" s="398" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="E38" s="399" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>241</v>
       </c>
-      <c r="B39" s="651" t="n">
+      <c r="B39" s="400" t="n">
         <v>-0.6</v>
       </c>
-      <c r="C39" t="s">
-        <v>249</v>
-      </c>
-      <c r="D39" t="n" s="652">
+      <c r="C39" s="38" t="s">
+        <v>248</v>
+      </c>
+      <c r="D39" s="401" t="n">
         <v>-0.08</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E39" s="402" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>243</v>
       </c>
-      <c r="B40" s="653" t="n">
+      <c r="B40" s="403" t="n">
+        <v>-0.05</v>
+      </c>
+      <c r="C40" s="39" t="s">
+        <v>248</v>
+      </c>
+      <c r="D40" s="404" t="n">
         <v>-0.03</v>
       </c>
-      <c r="C40" t="s">
-        <v>249</v>
-      </c>
-      <c r="D40" t="n" s="654">
-        <v>-0.01</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E40" s="405" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>86</v>
       </c>
-      <c r="B41" s="655" t="n">
-        <v>-0.16</v>
-      </c>
-      <c r="C41" t="n" s="656">
-        <v>-0.02</v>
-      </c>
-      <c r="D41" t="n" s="657">
-        <v>-0.01</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B41" s="406" t="n">
+        <v>-0.15</v>
+      </c>
+      <c r="C41" s="407" t="n">
+        <v>-0.03</v>
+      </c>
+      <c r="D41" s="408" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E41" s="409" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>88</v>
       </c>
-      <c r="B42" s="658" t="n">
-        <v>-0.3</v>
-      </c>
-      <c r="C42" t="n" s="659">
-        <v>-0.07</v>
-      </c>
-      <c r="D42" t="n" s="660">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B42" s="410" t="n">
+        <v>-0.31</v>
+      </c>
+      <c r="C42" s="411" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="D42" s="412" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E42" s="413" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>90</v>
       </c>
-      <c r="B43" s="661" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="C43" t="n" s="662">
+      <c r="B43" s="414" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="C43" s="415" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="D43" s="416" t="n">
+        <v>-0.04</v>
+      </c>
+      <c r="E43" s="417" t="n">
         <v>-0.01</v>
       </c>
-      <c r="D43" t="n" s="663">
-        <v>-0.03</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>92</v>
       </c>
-      <c r="B44" s="664" t="n">
+      <c r="B44" s="418" t="n">
         <v>-0.2</v>
       </c>
-      <c r="C44" t="n" s="665">
+      <c r="C44" s="419" t="n">
         <v>-0.07</v>
       </c>
-      <c r="D44" t="n" s="666">
+      <c r="D44" s="420" t="n">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E44" s="421" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>94</v>
       </c>
-      <c r="B45" s="667" t="n">
-        <v>-0.29</v>
-      </c>
-      <c r="C45" t="n" s="668">
-        <v>-0.02</v>
-      </c>
-      <c r="D45" t="n" s="669">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B45" s="422" t="n">
+        <v>-0.26</v>
+      </c>
+      <c r="C45" s="423" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D45" s="424" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="E45" s="425" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>96</v>
       </c>
-      <c r="B46" s="670" t="n">
-        <v>-0.06</v>
-      </c>
-      <c r="C46" t="n" s="671">
-        <v>0.03</v>
-      </c>
-      <c r="D46" t="n" s="672">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B46" s="426" t="n">
+        <v>-0.08</v>
+      </c>
+      <c r="C46" s="427" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D46" s="428" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E46" s="429" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>98</v>
       </c>
-      <c r="B47" s="673" t="n">
-        <v>-0.13</v>
-      </c>
-      <c r="C47" t="n" s="674">
+      <c r="B47" s="430" t="n">
+        <v>-0.15</v>
+      </c>
+      <c r="C47" s="431" t="n">
+        <v>-0.06</v>
+      </c>
+      <c r="D47" s="432" t="n">
+        <v>-0.04</v>
+      </c>
+      <c r="E47" s="433" t="n">
         <v>-0.01</v>
       </c>
-      <c r="D47" t="n" s="675">
-        <v>-0.01</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>100</v>
       </c>
-      <c r="B48" s="676" t="n">
-        <v>-0.41</v>
-      </c>
-      <c r="C48" t="n" s="677">
-        <v>-0.1</v>
-      </c>
-      <c r="D48" t="n" s="678">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B48" s="434" t="n">
+        <v>-0.39</v>
+      </c>
+      <c r="C48" s="435" t="n">
+        <v>-0.06</v>
+      </c>
+      <c r="D48" s="436" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="E48" s="437" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>102</v>
       </c>
-      <c r="B49" s="679" t="n">
-        <v>-0.4</v>
-      </c>
-      <c r="C49" t="n" s="680">
-        <v>-0.04</v>
-      </c>
-      <c r="D49" t="n" s="681">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="438" t="n">
+        <v>-0.36</v>
+      </c>
+      <c r="C49" s="439" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="D49" s="440" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="E49" s="441" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>104</v>
       </c>
-      <c r="B50" s="682" t="n">
-        <v>-0.18</v>
-      </c>
-      <c r="C50" t="n" s="683">
-        <v>0.01</v>
-      </c>
-      <c r="D50" t="n" s="684">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="442" t="n">
+        <v>-0.21</v>
+      </c>
+      <c r="C50" s="443" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="D50" s="444" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="E50" s="445" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>106</v>
       </c>
-      <c r="B51" s="685" t="n">
-        <v>-0.07</v>
-      </c>
-      <c r="C51" t="n" s="686">
+      <c r="B51" s="446" t="n">
+        <v>-0.08</v>
+      </c>
+      <c r="C51" s="447" t="n">
         <v>0.04</v>
       </c>
-      <c r="D51" t="n" s="687">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D51" s="448" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E51" s="449" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>10</v>
       </c>
-      <c r="B52" s="688" t="n">
+      <c r="B52" s="450" t="n">
         <v>-0.1</v>
       </c>
-      <c r="C52" t="n" s="689">
-        <v>-0.01</v>
-      </c>
-      <c r="D52" t="n" s="690">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52" s="451" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D52" s="452" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E52" s="453" t="n">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>109</v>
       </c>
-      <c r="B53" s="691" t="n">
+      <c r="B53" s="454" t="n">
         <v>0.01</v>
       </c>
-      <c r="C53" t="n" s="692">
-        <v>0.01</v>
-      </c>
-      <c r="D53" t="n" s="693">
+      <c r="C53" s="455" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D53" s="456" t="n">
         <v>-0.03</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E53" s="457" t="n">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>111</v>
       </c>
-      <c r="B54" s="694" t="n">
-        <v>-0.31</v>
-      </c>
-      <c r="C54" t="n" s="695">
-        <v>-0.07</v>
-      </c>
-      <c r="D54" t="n" s="696">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B54" s="458" t="n">
+        <v>-0.32</v>
+      </c>
+      <c r="C54" s="459" t="n">
+        <v>-0.05</v>
+      </c>
+      <c r="D54" s="460" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E54" s="461" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>113</v>
       </c>
-      <c r="B55" s="697" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="C55" t="n" s="698">
-        <v>0.08</v>
-      </c>
-      <c r="D55" t="n" s="699">
+      <c r="B55" s="462" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="C55" s="463" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="D55" s="464" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="E55" s="465" t="n">
         <v>0.01</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>115</v>
       </c>
-      <c r="B56" s="700" t="n">
+      <c r="B56" s="466" t="n">
         <v>-0.07</v>
       </c>
-      <c r="C56" t="n" s="701">
+      <c r="C56" s="467" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="D56" s="468" t="n">
         <v>0.01</v>
       </c>
-      <c r="D56" t="n" s="702">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E56" s="469" t="n">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>117</v>
       </c>
-      <c r="B57" s="703" t="n">
+      <c r="B57" s="470" t="n">
         <v>-0.07</v>
       </c>
-      <c r="C57" t="n" s="704">
-        <v>0.04</v>
-      </c>
-      <c r="D57" t="n" s="705">
+      <c r="C57" s="471" t="n">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D57" s="472" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E57" s="473" t="n">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>119</v>
       </c>
-      <c r="B58" s="706" t="n">
-        <v>-0.07</v>
-      </c>
-      <c r="C58" t="n" s="707">
-        <v>0.03</v>
-      </c>
-      <c r="D58" t="n" s="708">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B58" s="474" t="n">
+        <v>-0.05</v>
+      </c>
+      <c r="C58" s="475" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="D58" s="476" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E58" s="477" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>121</v>
       </c>
-      <c r="B59" s="709" t="n">
-        <v>-0.01</v>
-      </c>
-      <c r="C59" t="n" s="710">
+      <c r="B59" s="478" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="C59" s="479" t="n">
         <v>0.04</v>
       </c>
-      <c r="D59" t="n" s="711">
-        <v>-0.01</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D59" s="480" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="E59" s="481" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>123</v>
       </c>
-      <c r="B60" s="712" t="n">
-        <v>-0.26</v>
-      </c>
-      <c r="C60" t="n" s="713">
+      <c r="B60" s="482" t="n">
+        <v>-0.27</v>
+      </c>
+      <c r="C60" s="483" t="n">
         <v>-0.04</v>
       </c>
-      <c r="D60" t="n" s="714">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D60" s="484" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E60" s="485" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>125</v>
       </c>
-      <c r="B61" s="715" t="n">
+      <c r="B61" s="486" t="n">
         <v>-0.42</v>
       </c>
-      <c r="C61" t="n" s="716">
+      <c r="C61" s="487" t="n">
         <v>0.0</v>
       </c>
-      <c r="D61" t="n" s="717">
+      <c r="D61" s="488" t="n">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E61" s="489" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>127</v>
       </c>
-      <c r="B62" s="718" t="n">
-        <v>-0.03</v>
-      </c>
-      <c r="C62" t="n" s="719">
-        <v>0.03</v>
-      </c>
-      <c r="D62" t="n" s="720">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B62" s="490" t="n">
+        <v>-0.04</v>
+      </c>
+      <c r="C62" s="491" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D62" s="492" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E62" s="493" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>129</v>
       </c>
-      <c r="B63" s="721" t="n">
-        <v>-0.11</v>
-      </c>
-      <c r="C63" t="n" s="722">
-        <v>-0.03</v>
-      </c>
-      <c r="D63" t="n" s="723">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B63" s="494" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="C63" s="495" t="n">
+        <v>-0.05</v>
+      </c>
+      <c r="D63" s="496" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E63" s="497" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>131</v>
       </c>
-      <c r="B64" s="724" t="n">
-        <v>-0.28</v>
-      </c>
-      <c r="C64" t="n" s="725">
-        <v>-0.05</v>
-      </c>
-      <c r="D64" t="n" s="726">
-        <v>-0.01</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B64" s="498" t="n">
+        <v>-0.27</v>
+      </c>
+      <c r="C64" s="499" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D64" s="500" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E64" s="501" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>133</v>
       </c>
-      <c r="B65" s="727" t="n">
-        <v>-0.3</v>
-      </c>
-      <c r="C65" t="n" s="728">
+      <c r="B65" s="502" t="n">
+        <v>-0.31</v>
+      </c>
+      <c r="C65" s="503" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D65" s="504" t="n">
         <v>-0.01</v>
       </c>
-      <c r="D65" t="n" s="729">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E65" s="505" t="n">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>148</v>
       </c>
-      <c r="B66" s="730" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="C66" t="n" s="731">
-        <v>0.09</v>
-      </c>
-      <c r="D66" t="n" s="732">
+      <c r="B66" s="506" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="C66" s="507" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="D66" s="508" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="E66" s="509" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -5990,15 +7028,183 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="4.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="130.7109375" collapsed="true"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>246</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>248</v>
+      </c>
+      <c r="D2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C3" s="510" t="n">
+        <v>-0.20953846153846156</v>
+      </c>
+      <c r="D3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>265</v>
+      </c>
+      <c r="C4" s="511" t="n">
+        <v>-0.37333333333333335</v>
+      </c>
+      <c r="D4" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C5" s="512" t="n">
+        <v>-0.25333333333333335</v>
+      </c>
+      <c r="D5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>281</v>
+      </c>
+      <c r="C6" s="513" t="n">
+        <v>-0.01342857142857143</v>
+      </c>
+      <c r="D6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>261</v>
+      </c>
+      <c r="C7" s="514" t="n">
+        <v>-0.005384615384615385</v>
+      </c>
+      <c r="D7" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>248</v>
+      </c>
+      <c r="C8" t="s">
+        <v>248</v>
+      </c>
+      <c r="D8"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>269</v>
+      </c>
+      <c r="C9" t="s">
+        <v>248</v>
+      </c>
+      <c r="D9"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>258</v>
+      </c>
+      <c r="C10" s="515" t="n">
+        <v>-0.35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>270</v>
+      </c>
+      <c r="C11" s="516" t="n">
+        <v>0.005000000000000002</v>
+      </c>
+      <c r="D11" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>272</v>
+      </c>
+      <c r="C12" s="517" t="n">
+        <v>0.005000000000000002</v>
+      </c>
+      <c r="D12" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>248</v>
+      </c>
+      <c r="C13" t="s">
+        <v>248</v>
+      </c>
+      <c r="D13"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>274</v>
+      </c>
+      <c r="C14" t="s">
+        <v>248</v>
+      </c>
+      <c r="D14"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>275</v>
+      </c>
+      <c r="C15" s="518" t="n">
+        <v>-0.446</v>
+      </c>
+      <c r="D15" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>277</v>
+      </c>
+      <c r="C16" s="519" t="n">
+        <v>-0.46499999999999997</v>
+      </c>
+      <c r="D16" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="8">
+        <v>-0.21230769230769236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>